<commit_message>
BA test finalized and WebDriverManager added
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE20CD9-745C-4E5B-9F15-378D72C22214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9612EB3E-D4FE-47D9-8612-BC2B9E9F35CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D4FFD352-1B49-4A51-A5BA-3B6F341317D7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>BA_code</t>
   </si>
@@ -96,7 +96,7 @@
     <t>Nis</t>
   </si>
   <si>
-    <t>2551225255</t>
+    <t>Nish</t>
   </si>
 </sst>
 </file>
@@ -151,9 +151,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899AA46E-8FBC-4244-A5B8-6A2DCE7C63F5}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,144 +501,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>429</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3">
+        <v>432</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>420</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
+      <c r="K2" s="3">
+        <v>9876543210</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>5</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>12345</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>428</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="3">
+        <v>431</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>10</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>5</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3">
         <v>420</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
         <v>1234567890</v>
       </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
User section finished and some changes in BA section made
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9612EB3E-D4FE-47D9-8612-BC2B9E9F35CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2627A6C2-2A0C-4447-AF9E-F592FA8970BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D4FFD352-1B49-4A51-A5BA-3B6F341317D7}"/>
+    <workbookView xWindow="1944" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{D4FFD352-1B49-4A51-A5BA-3B6F341317D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -30,41 +30,178 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nishant Gore</author>
+  </authors>
+  <commentList>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{6C0A8E14-79DD-4153-A00D-93CA4ECED87D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New BA with valid data and active status
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{D82CA1A5-FF78-41F6-9AEE-E4D7804F1357}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New BA with invalid data
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{94D4C0EA-D0F6-4026-BE64-7E0E1981B704}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New BA with valid data and inactive status
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nishant Gore</author>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{0CE0E600-2E7C-46F5-A2D2-0A0584989AC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New user with valid data and active status
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{9102A71E-35C7-48AC-ADD8-576DA2C532BF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New user with valid data and inactive status
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{18C7A07E-5F18-4DB8-82C0-42872A710B23}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New user with invalid data
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
-  <si>
-    <t>BA_code</t>
-  </si>
-  <si>
-    <t>BA_Name</t>
-  </si>
-  <si>
-    <t>state_name</t>
-  </si>
-  <si>
-    <t>trade_discount</t>
-  </si>
-  <si>
-    <t>credit_period</t>
-  </si>
-  <si>
-    <t>trade_credit_period</t>
-  </si>
-  <si>
-    <t>ba_group_code</t>
-  </si>
-  <si>
-    <t>is_msmed</t>
-  </si>
-  <si>
-    <t>email_id</t>
-  </si>
-  <si>
-    <t>contact_person_name</t>
-  </si>
-  <si>
-    <t>contact_person_number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Nishant</t>
   </si>
@@ -97,13 +234,103 @@
   </si>
   <si>
     <t>Nish</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>BA Group ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>Gore</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>nishant@example.com</t>
+  </si>
+  <si>
+    <t>im+nishant</t>
+  </si>
+  <si>
+    <t>nis</t>
+  </si>
+  <si>
+    <t>InvalidName</t>
+  </si>
+  <si>
+    <t>InvalidLastName</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>itsnishant</t>
+  </si>
+  <si>
+    <t>Readonly</t>
+  </si>
+  <si>
+    <t>gore@gmail.com</t>
+  </si>
+  <si>
+    <t>imnishantg1</t>
+  </si>
+  <si>
+    <t>BA code</t>
+  </si>
+  <si>
+    <t>BA Name</t>
+  </si>
+  <si>
+    <t>State Name</t>
+  </si>
+  <si>
+    <t>Trade Discount</t>
+  </si>
+  <si>
+    <t>Credit Period</t>
+  </si>
+  <si>
+    <t>Trade Credit Period</t>
+  </si>
+  <si>
+    <t>BA Group Code</t>
+  </si>
+  <si>
+    <t>Is Msmed</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>Contact Person Name</t>
+  </si>
+  <si>
+    <t>Contact Person Number</t>
+  </si>
+  <si>
+    <t>gore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +354,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,11 +389,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -480,11 +722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899AA46E-8FBC-4244-A5B8-6A2DCE7C63F5}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899AA46E-8FBC-4244-A5B8-6A2DCE7C63F5}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,50 +742,50 @@
     <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>435</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>432</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="3">
         <v>10</v>
@@ -558,27 +800,27 @@
         <v>420</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="K2" s="3">
         <v>9876543210</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>429</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -593,27 +835,27 @@
         <v>420</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="K3" s="3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
         <v>10</v>
@@ -628,19 +870,19 @@
         <v>420</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K4" s="3">
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="K5" s="3"/>
     </row>
@@ -651,18 +893,117 @@
     <hyperlink ref="I4" r:id="rId3" xr:uid="{44FEB28B-6210-4E97-B9BE-E54684C52575}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC76102A-0FB2-4F50-9C9D-8432E18ED5ED}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC76102A-0FB2-4F50-9C9D-8432E18ED5ED}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{8DE7C7D0-B454-494F-9FCF-735534759446}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{7EC04953-1685-4861-93EA-357BB00B8E56}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{B1D8AFE2-BA48-4C06-ABC1-3E95074CFCD8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tax code finished and function to verify searched data added to testutils
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2627A6C2-2A0C-4447-AF9E-F592FA8970BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED483F-F859-40BE-A385-DFF115A9B7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1944" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{D4FFD352-1B49-4A51-A5BA-3B6F341317D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{D4FFD352-1B49-4A51-A5BA-3B6F341317D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>Nishant</t>
   </si>
@@ -324,6 +324,33 @@
   </si>
   <si>
     <t>gore</t>
+  </si>
+  <si>
+    <t>Tax Code</t>
+  </si>
+  <si>
+    <t>Tax Percent</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>INVALIDTC</t>
+  </si>
+  <si>
+    <t>invalidpercentage</t>
+  </si>
+  <si>
+    <t>Valid test data</t>
+  </si>
+  <si>
+    <t>Invalid test data</t>
+  </si>
+  <si>
+    <t>Update test data</t>
+  </si>
+  <si>
+    <t>ZC</t>
   </si>
 </sst>
 </file>
@@ -725,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899AA46E-8FBC-4244-A5B8-6A2DCE7C63F5}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1033,13 +1060,63 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF8A65F-D656-4ABB-84D0-A5AB807330D3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
data sheet modified and added to tests
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49387A0E-C8D9-46F4-8F42-4A529B3E1C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{D4FFD352-1B49-4A51-A5BA-3B6F341317D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="TaxCode" sheetId="6" r:id="rId6"/>
     <sheet name="Reason" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{6C0A8E14-79DD-4153-A00D-93CA4ECED87D}">
+    <comment ref="M2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{D82CA1A5-FF78-41F6-9AEE-E4D7804F1357}">
+    <comment ref="M3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{94D4C0EA-D0F6-4026-BE64-7E0E1981B704}">
+    <comment ref="M4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,12 +110,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{0CE0E600-2E7C-46F5-A2D2-0A0584989AC3}">
+    <comment ref="H2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{9102A71E-35C7-48AC-ADD8-576DA2C532BF}">
+    <comment ref="H3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{18C7A07E-5F18-4DB8-82C0-42872A710B23}">
+    <comment ref="H4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>Nishant</t>
   </si>
@@ -384,12 +378,30 @@
   </si>
   <si>
     <t>payment</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>customer_code</t>
+  </si>
+  <si>
+    <t>customer_period</t>
+  </si>
+  <si>
+    <t>customer_drop</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>AOB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -763,43 +775,80 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B651AE5-7351-4C74-A084-B987CD4EE71A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="4" width="16.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>2907657</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899AA46E-8FBC-4244-A5B8-6A2DCE7C63F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.54296875" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
+    <col min="11" max="11" width="26.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -948,9 +997,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{8D1F46EC-5EA7-46E4-BD3E-E9FA146C7F1B}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{6222D065-8258-440A-8781-024D4FC53F95}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{44FEB28B-6210-4E97-B9BE-E54684C52575}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId4"/>
@@ -958,21 +1007,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC76102A-0FB2-4F50-9C9D-8432E18ED5ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1057,9 +1106,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{8DE7C7D0-B454-494F-9FCF-735534759446}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{7EC04953-1685-4861-93EA-357BB00B8E56}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{B1D8AFE2-BA48-4C06-ABC1-3E95074CFCD8}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1068,42 +1117,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66200D79-537B-4861-9288-B135BECDE84F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55853A9C-D3D9-4201-BC62-A25C35F6095F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF8A65F-D656-4ABB-84D0-A5AB807330D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1154,17 +1203,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99184F0B-2F3C-404D-B71F-123CC4D625D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
all driver.findelement remove and utilies to generate random data and update excel sheet added
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0027EE6C-7D30-4535-B301-9CEF9DE4E2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="M2" authorId="0">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -110,12 +116,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -140,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -195,10 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
-  <si>
-    <t>Nishant</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="112">
   <si>
     <t>Medium</t>
   </si>
@@ -248,15 +251,9 @@
     <t>Email ID</t>
   </si>
   <si>
-    <t>Gore</t>
-  </si>
-  <si>
     <t>Commercial</t>
   </si>
   <si>
-    <t>nishant@example.com</t>
-  </si>
-  <si>
     <t>im+nishant</t>
   </si>
   <si>
@@ -272,18 +269,9 @@
     <t>Manager</t>
   </si>
   <si>
-    <t>itsnishant</t>
-  </si>
-  <si>
     <t>Readonly</t>
   </si>
   <si>
-    <t>gore@gmail.com</t>
-  </si>
-  <si>
-    <t>imnishantg1</t>
-  </si>
-  <si>
     <t>BA code</t>
   </si>
   <si>
@@ -317,9 +305,6 @@
     <t>Contact Person Number</t>
   </si>
   <si>
-    <t>gore</t>
-  </si>
-  <si>
     <t>Tax Code</t>
   </si>
   <si>
@@ -417,12 +402,148 @@
   </si>
   <si>
     <t>S4</t>
+  </si>
+  <si>
+    <t>(invalid name)</t>
+  </si>
+  <si>
+    <t>#invalid_code</t>
+  </si>
+  <si>
+    <t>gh</t>
+  </si>
+  <si>
+    <t>test_dqesin</t>
+  </si>
+  <si>
+    <t>test_bmfnmu</t>
+  </si>
+  <si>
+    <t>119217</t>
+  </si>
+  <si>
+    <t>389780</t>
+  </si>
+  <si>
+    <t>test_firstname1</t>
+  </si>
+  <si>
+    <t>test_firstname2</t>
+  </si>
+  <si>
+    <t>test_lastname1</t>
+  </si>
+  <si>
+    <t>test_lastname2</t>
+  </si>
+  <si>
+    <t>test_eiscsl</t>
+  </si>
+  <si>
+    <t>test_lbpunk</t>
+  </si>
+  <si>
+    <t>571388</t>
+  </si>
+  <si>
+    <t>312680</t>
+  </si>
+  <si>
+    <t>test_email1@gmail.com</t>
+  </si>
+  <si>
+    <t>test_email2@example.com</t>
+  </si>
+  <si>
+    <t>invalidemail@com</t>
+  </si>
+  <si>
+    <t>test_nkuusx</t>
+  </si>
+  <si>
+    <t>test_iimmhu</t>
+  </si>
+  <si>
+    <t>107426</t>
+  </si>
+  <si>
+    <t>991063</t>
+  </si>
+  <si>
+    <t>IK</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>test_eicjrdv</t>
+  </si>
+  <si>
+    <t>test_updated_szpgh</t>
+  </si>
+  <si>
+    <t>testcode_yboc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -796,54 +917,68 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375"/>
+    <col min="2" max="2" customWidth="true" width="15.21875"/>
+    <col min="3" max="3" customWidth="true" width="15.109375"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2">
+        <v>58</v>
+      </c>
+      <c r="B2" s="0">
         <v>2907657</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -852,70 +987,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="23.54296875" customWidth="1"/>
-    <col min="10" max="10" width="20.453125" customWidth="1"/>
-    <col min="11" max="11" width="26.36328125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="13.44140625"/>
+    <col min="4" max="4" customWidth="true" width="13.88671875"/>
+    <col min="5" max="5" customWidth="true" width="13.21875"/>
+    <col min="6" max="6" customWidth="true" width="17.77734375"/>
+    <col min="7" max="7" customWidth="true" width="13.88671875"/>
+    <col min="8" max="8" customWidth="true" width="12.0"/>
+    <col min="9" max="9" customWidth="true" width="23.5546875"/>
+    <col min="10" max="10" customWidth="true" width="20.44140625"/>
+    <col min="11" max="11" customWidth="true" width="26.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>435</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>5</v>
       </c>
       <c r="D2" s="3">
         <v>10</v>
@@ -929,14 +1064,14 @@
       <c r="G2" s="3">
         <v>420</v>
       </c>
-      <c r="H2" t="s">
-        <v>1</v>
+      <c r="H2" t="s" s="0">
+        <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s" s="0">
         <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
       </c>
       <c r="K2" s="3">
         <v>9876543210</v>
@@ -946,11 +1081,11 @@
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="B3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -964,28 +1099,28 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s">
-        <v>1</v>
+      <c r="H3" t="s" s="0">
+        <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
         <v>4</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>3</v>
       </c>
       <c r="K3" s="3">
         <v>12345</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>436</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+      <c r="A4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>6</v>
       </c>
       <c r="D4" s="3">
         <v>10</v>
@@ -999,14 +1134,14 @@
       <c r="G4" s="3">
         <v>420</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s" s="0">
         <v>8</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>9</v>
       </c>
       <c r="K4" s="3">
         <v>1234567890</v>
@@ -1018,9 +1153,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId4"/>
@@ -1028,108 +1163,108 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" customWidth="1"/>
-    <col min="6" max="6" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.109375"/>
+    <col min="2" max="2" customWidth="true" width="12.33203125"/>
+    <col min="3" max="3" customWidth="true" width="15.44140625"/>
+    <col min="4" max="4" customWidth="true" width="16.5546875"/>
+    <col min="5" max="5" customWidth="true" width="10.77734375"/>
+    <col min="6" max="6" customWidth="true" width="22.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>101</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F3" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="C4" t="s" s="0">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="E4" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1138,55 +1273,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="C2" s="0">
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C3" s="0">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>60</v>
+      <c r="D3" t="s" s="0">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1195,71 +1330,71 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.44140625"/>
+    <col min="2" max="2" customWidth="true" width="16.0"/>
+    <col min="3" max="3" customWidth="true" width="14.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1269,61 +1404,61 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
+    <col min="2" max="2" customWidth="true" width="18.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C3" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="0">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B4" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temporary commit to pull data from remote
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>Nishant</t>
   </si>
@@ -417,6 +417,24 @@
   </si>
   <si>
     <t>S4</t>
+  </si>
+  <si>
+    <t>4@</t>
+  </si>
+  <si>
+    <t>$$</t>
+  </si>
+  <si>
+    <t>_u</t>
+  </si>
+  <si>
+    <t>A@kk&amp;&amp;$$</t>
+  </si>
+  <si>
+    <t>&amp;&amp;$$%%</t>
+  </si>
+  <si>
+    <t>&amp;&amp;</t>
   </si>
 </sst>
 </file>
@@ -804,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -846,7 +864,24 @@
         <v>66</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1139,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,7 +1224,24 @@
         <v>60</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Code refactored in mdmDashboardpage some new test cases added in user and thread.sleep removed
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0027EE6C-7D30-4535-B301-9CEF9DE4E2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77698B3C-A7FC-4F59-839D-C84B2AA68A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -196,12 +196,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{85B40F72-5EFF-44E7-960C-B641BDADB5B8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New user with readonly status
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
   <si>
     <t>Medium</t>
   </si>
@@ -251,292 +276,259 @@
     <t>Email ID</t>
   </si>
   <si>
+    <t>im+nishant</t>
+  </si>
+  <si>
+    <t>nis</t>
+  </si>
+  <si>
+    <t>InvalidName</t>
+  </si>
+  <si>
+    <t>InvalidLastName</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Readonly</t>
+  </si>
+  <si>
+    <t>BA code</t>
+  </si>
+  <si>
+    <t>BA Name</t>
+  </si>
+  <si>
+    <t>State Name</t>
+  </si>
+  <si>
+    <t>Trade Discount</t>
+  </si>
+  <si>
+    <t>Credit Period</t>
+  </si>
+  <si>
+    <t>Trade Credit Period</t>
+  </si>
+  <si>
+    <t>BA Group Code</t>
+  </si>
+  <si>
+    <t>Is Msmed</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>Contact Person Name</t>
+  </si>
+  <si>
+    <t>Contact Person Number</t>
+  </si>
+  <si>
+    <t>Tax Code</t>
+  </si>
+  <si>
+    <t>Tax Percent</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>INVALIDTC</t>
+  </si>
+  <si>
+    <t>invalidpercentage</t>
+  </si>
+  <si>
+    <t>Valid test data</t>
+  </si>
+  <si>
+    <t>Invalid test data</t>
+  </si>
+  <si>
+    <t>Update test data</t>
+  </si>
+  <si>
+    <t>Reason Code</t>
+  </si>
+  <si>
+    <t>Reason Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>onhold</t>
+  </si>
+  <si>
+    <t>(invalid code)</t>
+  </si>
+  <si>
+    <t>(invalid reason)</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>updated_test_reason</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>customer_code</t>
+  </si>
+  <si>
+    <t>customer_period</t>
+  </si>
+  <si>
+    <t>customer_drop</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>AOB</t>
+  </si>
+  <si>
+    <t>tax_type</t>
+  </si>
+  <si>
+    <t>tax_code</t>
+  </si>
+  <si>
+    <t>tax_rate</t>
+  </si>
+  <si>
+    <t>tax_desp</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>invoices</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>(invalid name)</t>
+  </si>
+  <si>
+    <t>#invalid_code</t>
+  </si>
+  <si>
+    <t>gh</t>
+  </si>
+  <si>
+    <t>test_firstname1</t>
+  </si>
+  <si>
+    <t>test_firstname2</t>
+  </si>
+  <si>
+    <t>test_lastname1</t>
+  </si>
+  <si>
+    <t>test_lastname2</t>
+  </si>
+  <si>
+    <t>test_email1@gmail.com</t>
+  </si>
+  <si>
+    <t>test_email2@example.com</t>
+  </si>
+  <si>
+    <t>invalidemail@com</t>
+  </si>
+  <si>
+    <t>MDM</t>
+  </si>
+  <si>
+    <t>MLL</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>Company Code</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
     <t>Commercial</t>
   </si>
   <si>
-    <t>im+nishant</t>
-  </si>
-  <si>
-    <t>nis</t>
-  </si>
-  <si>
-    <t>InvalidName</t>
-  </si>
-  <si>
-    <t>InvalidLastName</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>Readonly</t>
-  </si>
-  <si>
-    <t>BA code</t>
-  </si>
-  <si>
-    <t>BA Name</t>
-  </si>
-  <si>
-    <t>State Name</t>
-  </si>
-  <si>
-    <t>Trade Discount</t>
-  </si>
-  <si>
-    <t>Credit Period</t>
-  </si>
-  <si>
-    <t>Trade Credit Period</t>
-  </si>
-  <si>
-    <t>BA Group Code</t>
-  </si>
-  <si>
-    <t>Is Msmed</t>
-  </si>
-  <si>
-    <t>Email Id</t>
-  </si>
-  <si>
-    <t>Contact Person Name</t>
-  </si>
-  <si>
-    <t>Contact Person Number</t>
-  </si>
-  <si>
-    <t>Tax Code</t>
-  </si>
-  <si>
-    <t>Tax Percent</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>INVALIDTC</t>
-  </si>
-  <si>
-    <t>invalidpercentage</t>
-  </si>
-  <si>
-    <t>Valid test data</t>
-  </si>
-  <si>
-    <t>Invalid test data</t>
-  </si>
-  <si>
-    <t>Update test data</t>
-  </si>
-  <si>
-    <t>ZC</t>
-  </si>
-  <si>
-    <t>Reason Code</t>
-  </si>
-  <si>
-    <t>Reason Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>test_reason</t>
-  </si>
-  <si>
-    <t>test_name</t>
-  </si>
-  <si>
-    <t>onhold</t>
-  </si>
-  <si>
-    <t>(invalid code)</t>
-  </si>
-  <si>
-    <t>(invalid reason)</t>
-  </si>
-  <si>
-    <t>temp</t>
-  </si>
-  <si>
-    <t>updated_test_reason</t>
-  </si>
-  <si>
-    <t>payment</t>
-  </si>
-  <si>
-    <t>customer_name</t>
-  </si>
-  <si>
-    <t>customer_code</t>
-  </si>
-  <si>
-    <t>customer_period</t>
-  </si>
-  <si>
-    <t>customer_drop</t>
-  </si>
-  <si>
-    <t>Akash</t>
-  </si>
-  <si>
-    <t>AOB</t>
-  </si>
-  <si>
-    <t>tax_type</t>
-  </si>
-  <si>
-    <t>tax_code</t>
-  </si>
-  <si>
-    <t>tax_rate</t>
-  </si>
-  <si>
-    <t>tax_desp</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>invoices</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>(invalid name)</t>
-  </si>
-  <si>
-    <t>#invalid_code</t>
-  </si>
-  <si>
-    <t>gh</t>
-  </si>
-  <si>
-    <t>test_dqesin</t>
-  </si>
-  <si>
-    <t>test_bmfnmu</t>
-  </si>
-  <si>
-    <t>119217</t>
-  </si>
-  <si>
-    <t>389780</t>
-  </si>
-  <si>
-    <t>test_firstname1</t>
-  </si>
-  <si>
-    <t>test_firstname2</t>
-  </si>
-  <si>
-    <t>test_lastname1</t>
-  </si>
-  <si>
-    <t>test_lastname2</t>
-  </si>
-  <si>
-    <t>test_eiscsl</t>
-  </si>
-  <si>
-    <t>test_lbpunk</t>
-  </si>
-  <si>
-    <t>571388</t>
-  </si>
-  <si>
-    <t>312680</t>
-  </si>
-  <si>
-    <t>test_email1@gmail.com</t>
-  </si>
-  <si>
-    <t>test_email2@example.com</t>
-  </si>
-  <si>
-    <t>invalidemail@com</t>
-  </si>
-  <si>
-    <t>test_nkuusx</t>
-  </si>
-  <si>
-    <t>test_iimmhu</t>
-  </si>
-  <si>
-    <t>107426</t>
-  </si>
-  <si>
-    <t>991063</t>
-  </si>
-  <si>
-    <t>IK</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>VI</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>JD</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>TL</t>
-  </si>
-  <si>
-    <t>28</t>
+    <t>test_firstname3</t>
+  </si>
+  <si>
+    <t>test_lastname3</t>
+  </si>
+  <si>
+    <t>test_lsxlne</t>
+  </si>
+  <si>
+    <t>test_zttvgv</t>
+  </si>
+  <si>
+    <t>test_zincts</t>
+  </si>
+  <si>
+    <t>744102</t>
+  </si>
+  <si>
+    <t>test_ewspdc</t>
+  </si>
+  <si>
+    <t>test_uyygup</t>
+  </si>
+  <si>
+    <t>605464</t>
+  </si>
+  <si>
+    <t>333210</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>47</t>
   </si>
   <si>
     <t>49</t>
   </si>
   <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>PK</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>PY</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>test_eicjrdv</t>
-  </si>
-  <si>
-    <t>test_updated_szpgh</t>
-  </si>
-  <si>
-    <t>testcode_yboc</t>
+    <t>test_beurbqg</t>
+  </si>
+  <si>
+    <t>test_updated_ejkpm</t>
+  </si>
+  <si>
+    <t>testcode_ngnr</t>
+  </si>
+  <si>
+    <t>test_byqbvj</t>
+  </si>
+  <si>
+    <t>test_xsnjbk</t>
+  </si>
+  <si>
+    <t>test_buawlc</t>
+  </si>
+  <si>
+    <t>465212</t>
+  </si>
+  <si>
+    <t>148899</t>
+  </si>
+  <si>
+    <t>007373</t>
   </si>
 </sst>
 </file>
@@ -941,21 +933,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0">
         <v>2907657</v>
@@ -964,21 +956,21 @@
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1009,45 +1001,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>5</v>
@@ -1114,10 +1106,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>6</v>
@@ -1164,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,10 +1169,12 @@
     <col min="3" max="3" customWidth="true" width="15.44140625"/>
     <col min="4" max="4" customWidth="true" width="16.5546875"/>
     <col min="5" max="5" customWidth="true" width="10.77734375"/>
-    <col min="6" max="6" customWidth="true" width="22.109375"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125"/>
+    <col min="7" max="7" customWidth="true" width="22.109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1199,76 +1193,112 @@
       <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>88</v>
+        <v>96</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="F4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="F5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{C6F9665F-75D9-4DF2-A29A-B78F30E4B8B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1284,44 +1314,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0">
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C3" s="0">
         <v>14</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1346,7 +1376,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,43 +1388,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>90</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>38</v>
-      </c>
       <c r="C3" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1419,46 +1449,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code refactored in PO based invoice submission page and new tests added
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932BD9EF-6408-4B58-B18E-FC0AA7B8BA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A717184-6D0D-4B03-94D4-80B9C43FF2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="157">
   <si>
     <t>Nishant</t>
   </si>
@@ -611,97 +611,103 @@
     <t>Nishant Gore</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>TESTINV3614</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>TESTINV6913</t>
+  </si>
+  <si>
+    <t>TESTINV7712</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0.8999999999999999</t>
+  </si>
+  <si>
+    <t>TESTINV1212</t>
+  </si>
+  <si>
+    <t>TESTINV1619</t>
+  </si>
+  <si>
+    <t>TESTINV4175</t>
+  </si>
+  <si>
+    <t>TESTINV3664</t>
+  </si>
+  <si>
+    <t>TESTINV9969</t>
+  </si>
+  <si>
+    <t>MANIPUR</t>
+  </si>
+  <si>
+    <t>TESTINV3712</t>
+  </si>
+  <si>
+    <t>TESTINV1887</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>TESTINV5595</t>
+  </si>
+  <si>
+    <t>TESTINV2223</t>
+  </si>
+  <si>
+    <t>TESTINV2561</t>
+  </si>
+  <si>
+    <t>TESTINV4211</t>
+  </si>
+  <si>
+    <t>TESTINV3819</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
     <t>1.44</t>
   </si>
   <si>
-    <t>TESTINV7193</t>
-  </si>
-  <si>
-    <t>TESTINV5306</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>TESTINV9119</t>
-  </si>
-  <si>
-    <t>TESTINV2453</t>
-  </si>
-  <si>
-    <t>TESTINV3846</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>TESTINV0310</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>TESTINV6373</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>TESTINV6974</t>
-  </si>
-  <si>
-    <t>PUNJAB</t>
-  </si>
-  <si>
-    <t>TESTINV8111</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>1.08</t>
-  </si>
-  <si>
-    <t>TESTINV5800</t>
-  </si>
-  <si>
-    <t>TESTINV2969</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0.36</t>
-  </si>
-  <si>
-    <t>TESTINV5338</t>
-  </si>
-  <si>
-    <t>TESTINV4770</t>
-  </si>
-  <si>
-    <t>TESTINV5144</t>
-  </si>
-  <si>
-    <t>TESTINV2290</t>
-  </si>
-  <si>
-    <t>TESTINV0851</t>
+    <t>TESTINV7271</t>
   </si>
 </sst>
 </file>
@@ -1691,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE238B9D-CDBF-41D9-8FEA-8D02BC451BAE}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1747,13 +1753,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>100</v>
@@ -1774,7 +1780,7 @@
         <v>112</v>
       </c>
       <c r="J2" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>122</v>
@@ -1788,10 +1794,10 @@
         <v>146</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>100</v>
@@ -1812,7 +1818,7 @@
         <v>113</v>
       </c>
       <c r="J3" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>122</v>
@@ -1823,13 +1829,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>100</v>
@@ -1850,7 +1856,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>122</v>
@@ -1864,10 +1870,10 @@
         <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>100</v>
@@ -1888,7 +1894,7 @@
         <v>115</v>
       </c>
       <c r="J5" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s" s="0">
         <v>122</v>
@@ -1902,10 +1908,10 @@
         <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>100</v>
@@ -1926,7 +1932,7 @@
         <v>116</v>
       </c>
       <c r="J6" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>122</v>
@@ -1940,10 +1946,10 @@
         <v>152</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>100</v>
@@ -1964,7 +1970,7 @@
         <v>117</v>
       </c>
       <c r="J7" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>122</v>
@@ -1978,10 +1984,10 @@
         <v>153</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>100</v>
@@ -2002,7 +2008,7 @@
         <v>118</v>
       </c>
       <c r="J8" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>122</v>
@@ -2013,13 +2019,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>100</v>
@@ -2040,7 +2046,7 @@
         <v>119</v>
       </c>
       <c r="J9" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K9" t="s" s="0">
         <v>122</v>
@@ -2060,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643F2239-1977-45CB-88D6-B3856414D647}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2083,7 +2089,7 @@
         <v>103</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
submitting po based invoice manually section finished
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A717184-6D0D-4B03-94D4-80B9C43FF2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD705AA-22F9-4294-80D8-CD0E8B92538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="155">
   <si>
     <t>Nishant</t>
   </si>
@@ -611,10 +611,28 @@
     <t>Nishant Gore</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>1.08</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1.44</t>
   </si>
   <si>
     <t>3</t>
@@ -623,91 +641,67 @@
     <t>0.54</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>TESTINV3614</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0.36</t>
-  </si>
-  <si>
-    <t>TESTINV6913</t>
-  </si>
-  <si>
-    <t>TESTINV7712</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>0.8999999999999999</t>
-  </si>
-  <si>
-    <t>TESTINV1212</t>
-  </si>
-  <si>
-    <t>TESTINV1619</t>
-  </si>
-  <si>
-    <t>TESTINV4175</t>
-  </si>
-  <si>
-    <t>TESTINV3664</t>
-  </si>
-  <si>
-    <t>TESTINV9969</t>
-  </si>
-  <si>
-    <t>MANIPUR</t>
-  </si>
-  <si>
-    <t>TESTINV3712</t>
-  </si>
-  <si>
-    <t>TESTINV1887</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
-    <t>TESTINV5595</t>
-  </si>
-  <si>
-    <t>TESTINV2223</t>
-  </si>
-  <si>
-    <t>TESTINV2561</t>
-  </si>
-  <si>
-    <t>TESTINV4211</t>
-  </si>
-  <si>
-    <t>TESTINV3819</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>1.44</t>
-  </si>
-  <si>
-    <t>TESTINV7271</t>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>TESTINV99432</t>
+  </si>
+  <si>
+    <t>TESTINV56488</t>
+  </si>
+  <si>
+    <t>TESTINV93601</t>
+  </si>
+  <si>
+    <t>TESTINV13609</t>
+  </si>
+  <si>
+    <t>TESTINV11826</t>
+  </si>
+  <si>
+    <t>TESTINV04404</t>
+  </si>
+  <si>
+    <t>TESTINV29186</t>
+  </si>
+  <si>
+    <t>TESTINV33221</t>
+  </si>
+  <si>
+    <t>TRIPURA</t>
+  </si>
+  <si>
+    <t>TESTINV24257</t>
+  </si>
+  <si>
+    <t>TESTINV70287</t>
+  </si>
+  <si>
+    <t>TESTINV07707</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>TESTINV49593</t>
+  </si>
+  <si>
+    <t>TESTINV87128</t>
+  </si>
+  <si>
+    <t>TESTINV79234</t>
+  </si>
+  <si>
+    <t>TESTINV09626</t>
+  </si>
+  <si>
+    <t>TESTINV34765</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE238B9D-CDBF-41D9-8FEA-8D02BC451BAE}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1756,10 +1750,10 @@
         <v>145</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>100</v>
@@ -1779,8 +1773,8 @@
       <c r="I2" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="J2" s="0">
-        <v>1</v>
+      <c r="J2" t="s" s="0">
+        <v>128</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>122</v>
@@ -1794,10 +1788,10 @@
         <v>146</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>100</v>
@@ -1817,8 +1811,8 @@
       <c r="I3" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="J3" s="0">
-        <v>1</v>
+      <c r="J3" t="s" s="0">
+        <v>130</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>122</v>
@@ -1829,13 +1823,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>149</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>128</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>129</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>100</v>
@@ -1855,8 +1849,8 @@
       <c r="I4" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="J4" s="0">
-        <v>1</v>
+      <c r="J4" t="s" s="0">
+        <v>148</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>122</v>
@@ -1870,10 +1864,10 @@
         <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>100</v>
@@ -1893,8 +1887,8 @@
       <c r="I5" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="J5" s="0">
-        <v>1</v>
+      <c r="J5" t="s" s="0">
+        <v>148</v>
       </c>
       <c r="K5" t="s" s="0">
         <v>122</v>
@@ -1908,10 +1902,10 @@
         <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>100</v>
@@ -1931,8 +1925,8 @@
       <c r="I6" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="J6" s="0">
-        <v>1</v>
+      <c r="J6" t="s" s="0">
+        <v>132</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>122</v>
@@ -1946,10 +1940,10 @@
         <v>152</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>100</v>
@@ -1969,8 +1963,8 @@
       <c r="I7" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="J7" s="0">
-        <v>1</v>
+      <c r="J7" t="s" s="0">
+        <v>130</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>122</v>
@@ -1984,10 +1978,10 @@
         <v>153</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>100</v>
@@ -2007,8 +2001,8 @@
       <c r="I8" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="J8" s="0">
-        <v>1</v>
+      <c r="J8" t="s" s="0">
+        <v>132</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>122</v>
@@ -2019,13 +2013,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s" s="0">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>100</v>
@@ -2045,8 +2039,8 @@
       <c r="I9" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="J9" s="0">
-        <v>1</v>
+      <c r="J9" t="s" s="0">
+        <v>128</v>
       </c>
       <c r="K9" t="s" s="0">
         <v>122</v>
@@ -2066,14 +2060,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643F2239-1977-45CB-88D6-B3856414D647}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="20.33203125"/>
-    <col min="2" max="2" customWidth="true" width="11.0"/>
+    <col min="2" max="2" customWidth="true" width="14.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tests added in po based invoice with excelsheet
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD705AA-22F9-4294-80D8-CD0E8B92538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B937DD27-6A94-47E6-AF2D-812105876CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="163">
   <si>
     <t>Nishant</t>
   </si>
@@ -611,10 +611,67 @@
     <t>Nishant Gore</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>0.72</t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1.44</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>TRIPURA</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>TESTINV58786</t>
+  </si>
+  <si>
+    <t>TESTINV68221</t>
+  </si>
+  <si>
+    <t>TESTINV29057</t>
+  </si>
+  <si>
+    <t>TESTINV58902</t>
+  </si>
+  <si>
+    <t>TESTINV45169</t>
+  </si>
+  <si>
+    <t>TESTINV82503</t>
+  </si>
+  <si>
+    <t>TESTINV10608</t>
+  </si>
+  <si>
+    <t>TESTINV20771</t>
+  </si>
+  <si>
+    <t>TESTINV94123</t>
+  </si>
+  <si>
+    <t>TESTINV18603</t>
   </si>
   <si>
     <t>1</t>
@@ -623,85 +680,52 @@
     <t>0.18</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>1.44</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>TESTINV99432</t>
-  </si>
-  <si>
-    <t>TESTINV56488</t>
-  </si>
-  <si>
-    <t>TESTINV93601</t>
-  </si>
-  <si>
-    <t>TESTINV13609</t>
-  </si>
-  <si>
-    <t>TESTINV11826</t>
-  </si>
-  <si>
-    <t>TESTINV04404</t>
-  </si>
-  <si>
-    <t>TESTINV29186</t>
-  </si>
-  <si>
-    <t>TESTINV33221</t>
-  </si>
-  <si>
-    <t>TRIPURA</t>
-  </si>
-  <si>
-    <t>TESTINV24257</t>
-  </si>
-  <si>
-    <t>TESTINV70287</t>
-  </si>
-  <si>
-    <t>TESTINV07707</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>1.62</t>
-  </si>
-  <si>
-    <t>TESTINV49593</t>
-  </si>
-  <si>
-    <t>TESTINV87128</t>
-  </si>
-  <si>
-    <t>TESTINV79234</t>
-  </si>
-  <si>
-    <t>TESTINV09626</t>
-  </si>
-  <si>
-    <t>TESTINV34765</t>
+    <t>TESTINV29856</t>
+  </si>
+  <si>
+    <t>TESTINV51736</t>
+  </si>
+  <si>
+    <t>TESTINV06441</t>
+  </si>
+  <si>
+    <t>TESTINV69104</t>
+  </si>
+  <si>
+    <t>TESTINV41715</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>TESTINV89525</t>
+  </si>
+  <si>
+    <t>TESTINV97192</t>
+  </si>
+  <si>
+    <t>TESTINV04156</t>
+  </si>
+  <si>
+    <t>TESTINV17714</t>
+  </si>
+  <si>
+    <t>TESTINV73341</t>
+  </si>
+  <si>
+    <t>TESTINV34048</t>
+  </si>
+  <si>
+    <t>TESTINV25913</t>
+  </si>
+  <si>
+    <t>TESTINV06532</t>
+  </si>
+  <si>
+    <t>TESTINV09872</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1716,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1747,13 +1771,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>100</v>
@@ -1774,7 +1798,7 @@
         <v>112</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>122</v>
@@ -1785,13 +1809,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>100</v>
@@ -1812,7 +1836,7 @@
         <v>113</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>122</v>
@@ -1823,13 +1847,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>100</v>
@@ -1850,7 +1874,7 @@
         <v>114</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>122</v>
@@ -1861,13 +1885,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>100</v>
@@ -1888,7 +1912,7 @@
         <v>115</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K5" t="s" s="0">
         <v>122</v>
@@ -1899,13 +1923,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>100</v>
@@ -1926,7 +1950,7 @@
         <v>116</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>122</v>
@@ -1937,13 +1961,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s" s="0">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>100</v>
@@ -1964,7 +1988,7 @@
         <v>117</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>122</v>
@@ -1975,13 +1999,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s" s="0">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>100</v>
@@ -2002,7 +2026,7 @@
         <v>118</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>122</v>
@@ -2013,13 +2037,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s" s="0">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>100</v>
@@ -2040,7 +2064,7 @@
         <v>119</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="K9" t="s" s="0">
         <v>122</v>
@@ -2058,16 +2082,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643F2239-1977-45CB-88D6-B3856414D647}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="20.33203125"/>
     <col min="2" max="2" customWidth="true" width="14.6640625"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875"/>
+    <col min="4" max="4" customWidth="true" width="14.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -2077,13 +2103,25 @@
       <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
         <v>103</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>144</v>
+        <v>130</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Tests added in po based invoice with excel sheet page
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B937DD27-6A94-47E6-AF2D-812105876CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23191D4-1A1F-4DD2-89B6-C3A395DAC503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="141">
   <si>
     <t>Nishant</t>
   </si>
@@ -611,12 +611,6 @@
     <t>Nishant Gore</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -629,81 +623,18 @@
     <t>0.54</t>
   </si>
   <si>
-    <t>TRIPURA</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>1.62</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
     <t>0.36</t>
   </si>
   <si>
-    <t>TESTINV58786</t>
-  </si>
-  <si>
-    <t>TESTINV68221</t>
-  </si>
-  <si>
-    <t>TESTINV29057</t>
-  </si>
-  <si>
-    <t>TESTINV58902</t>
-  </si>
-  <si>
-    <t>TESTINV45169</t>
-  </si>
-  <si>
-    <t>TESTINV82503</t>
-  </si>
-  <si>
-    <t>TESTINV10608</t>
-  </si>
-  <si>
-    <t>TESTINV20771</t>
-  </si>
-  <si>
-    <t>TESTINV94123</t>
-  </si>
-  <si>
-    <t>TESTINV18603</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>0.18</t>
   </si>
   <si>
-    <t>TESTINV29856</t>
-  </si>
-  <si>
-    <t>TESTINV51736</t>
-  </si>
-  <si>
-    <t>TESTINV06441</t>
-  </si>
-  <si>
-    <t>TESTINV69104</t>
-  </si>
-  <si>
-    <t>TESTINV41715</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>1.08</t>
-  </si>
-  <si>
-    <t>TESTINV89525</t>
-  </si>
-  <si>
     <t>TESTINV97192</t>
   </si>
   <si>
@@ -726,13 +657,15 @@
   </si>
   <si>
     <t>TESTINV09872</t>
+  </si>
+  <si>
+    <t>PONDICHERRY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1128,10 +1061,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375"/>
-    <col min="2" max="2" customWidth="true" width="15.21875"/>
-    <col min="3" max="3" customWidth="true" width="15.109375"/>
-    <col min="4" max="4" customWidth="true" width="16.88671875"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1152,10 +1085,10 @@
       <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1166,13 +1099,13 @@
       <c r="A3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>77</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1186,7 +1119,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1194,15 +1127,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.44140625"/>
-    <col min="4" max="4" customWidth="true" width="13.88671875"/>
-    <col min="5" max="5" customWidth="true" width="13.21875"/>
-    <col min="6" max="6" customWidth="true" width="17.77734375"/>
-    <col min="7" max="7" customWidth="true" width="13.88671875"/>
-    <col min="8" max="8" customWidth="true" width="12.0"/>
-    <col min="9" max="9" customWidth="true" width="23.5546875"/>
-    <col min="10" max="10" customWidth="true" width="20.44140625"/>
-    <col min="11" max="11" customWidth="true" width="26.33203125"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1244,10 +1177,10 @@
       <c r="A2" s="3">
         <v>435</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3">
@@ -1262,13 +1195,13 @@
       <c r="G2" s="3">
         <v>420</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="3">
@@ -1279,10 +1212,10 @@
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3">
@@ -1297,13 +1230,13 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>4</v>
       </c>
       <c r="K3" s="3">
@@ -1314,10 +1247,10 @@
       <c r="A4" s="3">
         <v>436</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3">
@@ -1332,13 +1265,13 @@
       <c r="G4" s="3">
         <v>420</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="3">
@@ -1362,7 +1295,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -1370,12 +1303,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.109375"/>
-    <col min="2" max="2" customWidth="true" width="12.33203125"/>
-    <col min="3" max="3" customWidth="true" width="10.6640625"/>
-    <col min="4" max="4" customWidth="true" width="16.5546875"/>
-    <col min="5" max="5" customWidth="true" width="10.77734375"/>
-    <col min="6" max="6" customWidth="true" width="22.109375"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1399,19 +1332,19 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>101</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1419,19 +1352,19 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>102</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1439,19 +1372,19 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -1498,10 +1431,10 @@
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1509,16 +1442,16 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>14</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1526,13 +1459,13 @@
       <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1554,7 +1487,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.21875"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1566,18 +1499,18 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1596,9 +1529,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.44140625"/>
-    <col min="2" max="2" customWidth="true" width="16.0"/>
-    <col min="3" max="3" customWidth="true" width="14.21875"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1613,32 +1546,32 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="0">
+      <c r="B4">
         <v>13</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1658,8 +1591,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
-    <col min="2" max="2" customWidth="true" width="18.77734375"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1674,35 +1607,35 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1721,14 +1654,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875"/>
-    <col min="4" max="4" customWidth="true" width="19.6640625"/>
-    <col min="7" max="7" customWidth="true" width="10.33203125"/>
-    <col min="8" max="8" customWidth="true" width="16.77734375"/>
-    <col min="9" max="9" customWidth="true" width="16.88671875"/>
-    <col min="11" max="11" customWidth="true" width="13.6640625"/>
-    <col min="12" max="12" customWidth="true" width="15.21875"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1770,306 +1703,306 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>155</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>996713</v>
+      </c>
+      <c r="H2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>996713</v>
+      </c>
+      <c r="H3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>996713</v>
+      </c>
+      <c r="H4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>996713</v>
+      </c>
+      <c r="H5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>996713</v>
+      </c>
+      <c r="H6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C7" t="s">
         <v>127</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D7" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="0">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0">
-        <v>1</v>
-      </c>
-      <c r="G2" s="0">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>996713</v>
       </c>
-      <c r="H2" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>112</v>
-      </c>
-      <c r="J2" t="s" s="0">
+      <c r="H7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" t="s">
         <v>126</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K7" t="s">
         <v>122</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
-        <v>156</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>126</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>127</v>
-      </c>
-      <c r="D3" t="s" s="0">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F8">
         <v>0</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G8">
         <v>996713</v>
       </c>
-      <c r="H3" t="s" s="0">
-        <v>105</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>126</v>
-      </c>
-      <c r="K3" t="s" s="0">
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K8" t="s">
         <v>122</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>126</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>127</v>
-      </c>
-      <c r="D4" t="s" s="0">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G9">
         <v>996713</v>
       </c>
-      <c r="H4" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>114</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>126</v>
-      </c>
-      <c r="K4" t="s" s="0">
+      <c r="H9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" t="s">
+        <v>119</v>
+      </c>
+      <c r="J9" t="s">
+        <v>128</v>
+      </c>
+      <c r="K9" t="s">
         <v>122</v>
       </c>
-      <c r="L4" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
-        <v>158</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>146</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="E5" s="0">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>115</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="K5" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="L5" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
-        <v>159</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>134</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="E6" s="0">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>116</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="K6" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
-        <v>160</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>128</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>129</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="E7" s="0">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>117</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>128</v>
-      </c>
-      <c r="K7" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
-        <v>161</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>146</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="E8" s="0">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>118</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="K8" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="L8" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
-        <v>162</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>134</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="E9" s="0">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>119</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="K9" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="L9" t="s" s="0">
+      <c r="L9" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2082,18 +2015,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643F2239-1977-45CB-88D6-B3856414D647}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.33203125"/>
-    <col min="2" max="2" customWidth="true" width="14.6640625"/>
-    <col min="3" max="3" customWidth="true" width="15.5546875"/>
-    <col min="4" max="4" customWidth="true" width="14.44140625"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -2111,16 +2044,16 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
         <v>122</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fitler section review done
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Reason" sheetId="7" r:id="rId7"/>
     <sheet name="POBasedInvoice" sheetId="8" r:id="rId8"/>
     <sheet name="BADashboardPage" sheetId="9" r:id="rId9"/>
+    <sheet name="CommercialDashboardPage" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -231,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="155">
   <si>
     <t>Nishant</t>
   </si>
@@ -665,23 +666,44 @@
     <t>Memo number</t>
   </si>
   <si>
+    <t>TESTINV07707</t>
+  </si>
+  <si>
+    <t>Location Name</t>
+  </si>
+  <si>
+    <t>Ahmedabad (MLL)</t>
+  </si>
+  <si>
+    <t>30005631-2023-24-00019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company </t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>Cargo Handling</t>
+  </si>
+  <si>
     <t>30005631-2023-24-00009</t>
-  </si>
-  <si>
-    <t>TESTINV07707</t>
-  </si>
-  <si>
-    <t>Location Name</t>
-  </si>
-  <si>
-    <t>Ahmedabad (MLL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -724,6 +746,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -746,13 +774,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1074,7 +1105,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
     <col min="2" max="2" width="15.21875" customWidth="1"/>
@@ -1082,7 +1113,7 @@
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -1096,7 +1127,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
@@ -1110,7 +1141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
         <v>75</v>
       </c>
@@ -1129,6 +1160,62 @@
     <hyperlink ref="A3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1022</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1140,7 +1227,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" customWidth="1"/>
@@ -1153,7 +1240,7 @@
     <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1188,7 +1275,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" s="3">
         <v>435</v>
       </c>
@@ -1223,7 +1310,7 @@
         <v>9876543210</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" s="3">
         <v>429</v>
       </c>
@@ -1258,7 +1345,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" s="3">
         <v>436</v>
       </c>
@@ -1293,7 +1380,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="3"/>
       <c r="K5" s="3"/>
     </row>
@@ -1316,7 +1403,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
@@ -1326,7 +1413,7 @@
     <col min="6" max="6" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1366,7 +1453,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1386,7 +1473,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1426,9 +1513,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -1442,7 +1529,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
@@ -1456,7 +1543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1470,7 +1557,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
@@ -1500,12 +1587,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
@@ -1513,7 +1600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1521,7 +1608,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -1542,14 +1629,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -1560,7 +1647,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1571,7 +1658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1582,7 +1669,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="B4">
         <v>13</v>
       </c>
@@ -1604,13 +1691,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -1621,7 +1708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1632,7 +1719,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1643,7 +1730,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1667,7 +1754,7 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" customWidth="1"/>
@@ -1679,7 +1766,7 @@
     <col min="12" max="12" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1717,7 +1804,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -1755,7 +1842,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -1793,7 +1880,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -1831,7 +1918,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -1869,7 +1956,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -1907,7 +1994,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -1945,7 +2032,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>138</v>
       </c>
@@ -1983,7 +2070,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>139</v>
       </c>
@@ -2032,11 +2119,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -2049,7 +2136,7 @@
     <col min="9" max="9" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -2075,10 +2162,10 @@
         <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -2098,13 +2185,13 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
         <v>144</v>
       </c>
-      <c r="H2" t="s">
-        <v>145</v>
-      </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated billtestdata and config.properties and fixed issues in poBasedInvoiceAck page
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5058AA76-EE22-41FE-BCB3-D8B467D43D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0A763-D17A-492A-9AE7-F6CD672C8CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="257">
   <si>
     <t>Medium</t>
   </si>
@@ -745,9 +745,6 @@
     <t>Update test data</t>
   </si>
   <si>
-    <t>ZC</t>
-  </si>
-  <si>
     <t>Reason Code</t>
   </si>
   <si>
@@ -844,15 +841,6 @@
     <t>810948</t>
   </si>
   <si>
-    <t>test_jortske</t>
-  </si>
-  <si>
-    <t>test_updated_fagsp</t>
-  </si>
-  <si>
-    <t>testcode_yjbz</t>
-  </si>
-  <si>
     <t>Role name</t>
   </si>
   <si>
@@ -970,343 +958,442 @@
     <t>3</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>PONDICHERRY</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Service name</t>
+  </si>
+  <si>
+    <t>Memo number</t>
+  </si>
+  <si>
+    <t>TESTINV07707</t>
+  </si>
+  <si>
+    <t>Location Name</t>
+  </si>
+  <si>
+    <t>Ahmedabad (MLL)</t>
+  </si>
+  <si>
+    <t>30005631-2023-24-00019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company </t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>Cargo Handling</t>
+  </si>
+  <si>
+    <t>30005631-2023-24-00009</t>
+  </si>
+  <si>
+    <t>suraj suraj</t>
+  </si>
+  <si>
+    <t>company_code</t>
+  </si>
+  <si>
+    <t>service_type</t>
+  </si>
+  <si>
+    <t>MLL - 1022</t>
+  </si>
+  <si>
+    <t>GENERAL EXPENSES</t>
+  </si>
+  <si>
+    <t>MERU - MLMO</t>
+  </si>
+  <si>
+    <t>MESPL - MESP</t>
+  </si>
+  <si>
+    <t>#####</t>
+  </si>
+  <si>
+    <t>####</t>
+  </si>
+  <si>
+    <t>MAHARASHTRA - 300005574</t>
+  </si>
+  <si>
+    <t>NAGALAND</t>
+  </si>
+  <si>
+    <t>DELHI</t>
+  </si>
+  <si>
+    <t>TESTINV2040</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>TESTINV9711</t>
+  </si>
+  <si>
+    <t>TESTINV2439</t>
+  </si>
+  <si>
+    <t>TESTINV6823</t>
+  </si>
+  <si>
+    <t>TESTINV9107</t>
+  </si>
+  <si>
+    <t>TESTINV6572</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>TESTINV8622</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>TESTINV9890</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>594194</t>
+  </si>
+  <si>
+    <t>616938</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Reject reason</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Item text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitting From </t>
+  </si>
+  <si>
+    <t>Batch Id</t>
+  </si>
+  <si>
+    <t>Verified By</t>
+  </si>
+  <si>
+    <t>30005631-2023-24-00008</t>
+  </si>
+  <si>
+    <t>TESTINV84279</t>
+  </si>
+  <si>
+    <t>Agreement not available</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Suraj Suraj</t>
+  </si>
+  <si>
+    <t>30005631-2023-24-00031</t>
+  </si>
+  <si>
+    <t>TESTINV90004</t>
+  </si>
+  <si>
+    <t>anusha logi</t>
+  </si>
+  <si>
+    <t>T-20005329-13Mar2024@09:40:55</t>
+  </si>
+  <si>
+    <t>T-20005329-13Mar2024@09:40:54</t>
+  </si>
+  <si>
+    <t>30005631-2023-24-00016</t>
+  </si>
+  <si>
+    <t>Transactional data mismatch</t>
+  </si>
+  <si>
+    <t>#$*/()</t>
+  </si>
+  <si>
+    <t>invalid_Baname</t>
+  </si>
+  <si>
+    <t>test_iqidek</t>
+  </si>
+  <si>
+    <t>test_ixhpgj</t>
+  </si>
+  <si>
+    <t>308645</t>
+  </si>
+  <si>
+    <t>726605</t>
+  </si>
+  <si>
+    <t>Company Code</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>MLL</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>MDM</t>
+  </si>
+  <si>
+    <t>testemail@gmail.com</t>
+  </si>
+  <si>
+    <t>test_kmrahi</t>
+  </si>
+  <si>
+    <t>test_cnthne</t>
+  </si>
+  <si>
+    <t>test_odxlxy</t>
+  </si>
+  <si>
+    <t>851517</t>
+  </si>
+  <si>
+    <t>382474</t>
+  </si>
+  <si>
+    <t>214129</t>
+  </si>
+  <si>
+    <t>test_first_name_1</t>
+  </si>
+  <si>
+    <t>test_last_name_1</t>
+  </si>
+  <si>
+    <t>test_first_name_2</t>
+  </si>
+  <si>
+    <t>test_last_name_2</t>
+  </si>
+  <si>
+    <t>test_last_name_3</t>
+  </si>
+  <si>
+    <t>test_last_name_4</t>
+  </si>
+  <si>
+    <t>test_first_name_3</t>
+  </si>
+  <si>
+    <t>test_first_name_4</t>
+  </si>
+  <si>
+    <t>XC</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>test_qgwymqj</t>
+  </si>
+  <si>
+    <t>test_updated_hkoiu</t>
+  </si>
+  <si>
+    <t>testcode_xmwt</t>
+  </si>
+  <si>
+    <t>TESTINV45388</t>
+  </si>
+  <si>
+    <t>TESTINV02796</t>
+  </si>
+  <si>
+    <t>TESTINV41933</t>
+  </si>
+  <si>
+    <t>TESTINV76157</t>
+  </si>
+  <si>
+    <t>TESTINV49001</t>
+  </si>
+  <si>
+    <t>TESTINV45851</t>
+  </si>
+  <si>
+    <t>TESTINV13480</t>
+  </si>
+  <si>
+    <t>TESTINV62709</t>
+  </si>
+  <si>
+    <t>TESTINV78658</t>
+  </si>
+  <si>
+    <t>TESTINV88778</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>TESTINV43920</t>
+  </si>
+  <si>
+    <t>TESTINV76112</t>
+  </si>
+  <si>
+    <t>TESTINV06328</t>
+  </si>
+  <si>
+    <t>TESTINV80545</t>
+  </si>
+  <si>
+    <t>TESTINV97856</t>
+  </si>
+  <si>
+    <t>TESTINV60190</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>TESTINV05801</t>
+  </si>
+  <si>
+    <t>TESTINV16282</t>
+  </si>
+  <si>
+    <t>TESTINV26832</t>
+  </si>
+  <si>
+    <t>TESTINV64392</t>
+  </si>
+  <si>
+    <t>TESTINV32156</t>
+  </si>
+  <si>
+    <t>TESTINV95278</t>
+  </si>
+  <si>
+    <t>TESTINV08439</t>
+  </si>
+  <si>
+    <t>TESTINV92737</t>
+  </si>
+  <si>
+    <t>TESTINV88822</t>
+  </si>
+  <si>
     <t>0.54</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0.36</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>TESTINV97192</t>
-  </si>
-  <si>
-    <t>TESTINV04156</t>
-  </si>
-  <si>
-    <t>TESTINV17714</t>
-  </si>
-  <si>
-    <t>TESTINV73341</t>
-  </si>
-  <si>
-    <t>TESTINV34048</t>
-  </si>
-  <si>
-    <t>TESTINV25913</t>
-  </si>
-  <si>
-    <t>TESTINV06532</t>
-  </si>
-  <si>
-    <t>TESTINV09872</t>
-  </si>
-  <si>
-    <t>PONDICHERRY</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Service name</t>
-  </si>
-  <si>
-    <t>Memo number</t>
-  </si>
-  <si>
-    <t>TESTINV07707</t>
-  </si>
-  <si>
-    <t>Location Name</t>
-  </si>
-  <si>
-    <t>Ahmedabad (MLL)</t>
-  </si>
-  <si>
-    <t>30005631-2023-24-00019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Company </t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>Memo</t>
-  </si>
-  <si>
-    <t>Cargo Handling</t>
-  </si>
-  <si>
-    <t>30005631-2023-24-00009</t>
-  </si>
-  <si>
-    <t>suraj suraj</t>
-  </si>
-  <si>
-    <t>company_code</t>
-  </si>
-  <si>
-    <t>service_type</t>
-  </si>
-  <si>
-    <t>MLL - 1022</t>
-  </si>
-  <si>
-    <t>GENERAL EXPENSES</t>
-  </si>
-  <si>
-    <t>MERU - MLMO</t>
-  </si>
-  <si>
-    <t>MESPL - MESP</t>
-  </si>
-  <si>
-    <t>#####</t>
-  </si>
-  <si>
-    <t>####</t>
-  </si>
-  <si>
-    <t>MAHARASHTRA - 300005574</t>
-  </si>
-  <si>
-    <t>NAGALAND</t>
-  </si>
-  <si>
-    <t>DELHI</t>
-  </si>
-  <si>
-    <t>TESTINV2040</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>TESTINV9711</t>
-  </si>
-  <si>
-    <t>TESTINV2439</t>
-  </si>
-  <si>
-    <t>TESTINV6823</t>
-  </si>
-  <si>
-    <t>TESTINV9107</t>
-  </si>
-  <si>
-    <t>TESTINV6572</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
-    <t>TESTINV8622</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>1.08</t>
-  </si>
-  <si>
-    <t>TESTINV9890</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>594194</t>
-  </si>
-  <si>
-    <t>616938</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Reject reason</t>
-  </si>
-  <si>
-    <t>Assignment</t>
-  </si>
-  <si>
-    <t>Item text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submitting From </t>
-  </si>
-  <si>
-    <t>Batch Id</t>
-  </si>
-  <si>
-    <t>Verified By</t>
-  </si>
-  <si>
-    <t>30005631-2023-24-00008</t>
-  </si>
-  <si>
-    <t>TESTINV84279</t>
-  </si>
-  <si>
-    <t>Agreement not available</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Suraj Suraj</t>
-  </si>
-  <si>
-    <t>30005631-2023-24-00031</t>
-  </si>
-  <si>
-    <t>TESTINV90004</t>
-  </si>
-  <si>
-    <t>anusha logi</t>
-  </si>
-  <si>
-    <t>T-20005329-13Mar2024@09:40:55</t>
-  </si>
-  <si>
-    <t>T-20005329-13Mar2024@09:40:54</t>
-  </si>
-  <si>
-    <t>30005631-2023-24-00016</t>
-  </si>
-  <si>
-    <t>Transactional data mismatch</t>
-  </si>
-  <si>
-    <t>#$*/()</t>
-  </si>
-  <si>
-    <t>invalid_Baname</t>
-  </si>
-  <si>
-    <t>test_iqidek</t>
-  </si>
-  <si>
-    <t>test_ixhpgj</t>
-  </si>
-  <si>
-    <t>308645</t>
-  </si>
-  <si>
-    <t>726605</t>
-  </si>
-  <si>
-    <t>Company Code</t>
-  </si>
-  <si>
-    <t>City Name</t>
-  </si>
-  <si>
-    <t>MLL</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>MDM</t>
-  </si>
-  <si>
-    <t>testemail@gmail.com</t>
-  </si>
-  <si>
-    <t>test_kmrahi</t>
-  </si>
-  <si>
-    <t>test_cnthne</t>
-  </si>
-  <si>
-    <t>test_odxlxy</t>
-  </si>
-  <si>
-    <t>851517</t>
-  </si>
-  <si>
-    <t>382474</t>
-  </si>
-  <si>
-    <t>214129</t>
-  </si>
-  <si>
-    <t>test_first_name_1</t>
-  </si>
-  <si>
-    <t>test_last_name_1</t>
-  </si>
-  <si>
-    <t>test_first_name_2</t>
-  </si>
-  <si>
-    <t>test_last_name_2</t>
-  </si>
-  <si>
-    <t>test_last_name_3</t>
-  </si>
-  <si>
-    <t>test_last_name_4</t>
-  </si>
-  <si>
-    <t>test_first_name_3</t>
-  </si>
-  <si>
-    <t>test_first_name_4</t>
-  </si>
-  <si>
-    <t>QH</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>XC</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>test_qgwymqj</t>
-  </si>
-  <si>
-    <t>test_updated_hkoiu</t>
-  </si>
-  <si>
-    <t>testcode_xmwt</t>
+    <t>TESTINV92552</t>
+  </si>
+  <si>
+    <t>TESTINV77709</t>
+  </si>
+  <si>
+    <t>TESTINV34200</t>
+  </si>
+  <si>
+    <t>TESTINV43542</t>
+  </si>
+  <si>
+    <t>TESTINV45240</t>
+  </si>
+  <si>
+    <t>TESTINV42823</t>
+  </si>
+  <si>
+    <t>TESTINV84545</t>
+  </si>
+  <si>
+    <t>TESTINV64940</t>
+  </si>
+  <si>
+    <t>TESTINV02644</t>
+  </si>
+  <si>
+    <t>TESTINV03865</t>
+  </si>
+  <si>
+    <t>TESTINV39963</t>
+  </si>
+  <si>
+    <t>TESTINV48911</t>
+  </si>
+  <si>
+    <t>TESTINV71542</t>
+  </si>
+  <si>
+    <t>TESTINV17489</t>
+  </si>
+  <si>
+    <t>TESTINV19684</t>
   </si>
 </sst>
 </file>
@@ -1793,58 +1880,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C2" s="0">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>68</v>
-      </c>
       <c r="D3" t="s" s="0">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s" s="0">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C4" s="0">
         <v>12</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1878,117 +1965,117 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s" s="0">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E2" s="0">
         <v>1022</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s" s="0">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s" s="0">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s" s="0">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2015,19 +2102,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2035,16 +2122,16 @@
         <v>1022</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2071,60 +2158,60 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s" s="0">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E2" s="0">
         <v>0</v>
@@ -2136,39 +2223,39 @@
         <v>996713</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s" s="0">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E3" s="0">
         <v>0</v>
@@ -2180,39 +2267,39 @@
         <v>996713</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s" s="0">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E4" s="0">
         <v>0</v>
@@ -2224,39 +2311,39 @@
         <v>996713</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s" s="0">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
@@ -2268,39 +2355,39 @@
         <v>996713</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s" s="0">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E6" s="0">
         <v>0</v>
@@ -2312,39 +2399,39 @@
         <v>996713</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s" s="0">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E7" s="0">
         <v>0</v>
@@ -2356,39 +2443,39 @@
         <v>996713</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M7" t="s" s="0">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s" s="0">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E8" s="0">
         <v>0</v>
@@ -2400,39 +2487,39 @@
         <v>996713</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="K8" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="J8" t="s" s="0">
-        <v>118</v>
-      </c>
-      <c r="K8" t="s" s="0">
-        <v>110</v>
-      </c>
       <c r="L8" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M8" t="s" s="0">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="N8" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s" s="0">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E9" s="0">
         <v>0</v>
@@ -2444,25 +2531,25 @@
         <v>996713</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L9" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2494,322 +2581,322 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="7" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s" s="0">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s" s="0">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s" s="0">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s" s="0">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
       <c r="A8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="J10" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2876,10 +2963,10 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>5</v>
@@ -2946,10 +3033,10 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>6</v>
@@ -2998,7 +3085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
@@ -3033,62 +3120,62 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s" s="0">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s" s="0">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3099,10 +3186,10 @@
         <v>18</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>19</v>
@@ -3111,36 +3198,36 @@
         <v>4</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s" s="0">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -3169,58 +3256,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>172</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>173</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s" s="0">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0">
         <v>14</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>64</v>
-      </c>
       <c r="D4" t="s" s="0">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3246,26 +3333,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>71</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>69</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3301,10 +3388,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s" s="0">
-        <v>222</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>223</v>
+        <v>206</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>207</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>37</v>
@@ -3322,8 +3409,8 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="0" t="s">
-        <v>224</v>
+      <c r="B4" t="s" s="0">
+        <v>208</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>39</v>
@@ -3351,46 +3438,46 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s" s="0">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
         <v>46</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>48</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>226</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -3402,8 +3489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3420,92 +3507,92 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s" s="0">
-        <v>120</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>112</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="0">
         <v>996713</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>112</v>
+        <v>222</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s" s="0">
-        <v>121</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E3" s="0">
         <v>0</v>
@@ -3517,33 +3604,33 @@
         <v>996713</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s" s="0">
-        <v>122</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E4" s="0">
         <v>0</v>
@@ -3555,33 +3642,33 @@
         <v>996713</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s" s="0">
-        <v>123</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
@@ -3593,33 +3680,33 @@
         <v>996713</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s" s="0">
-        <v>124</v>
+        <v>253</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E6" s="0">
         <v>0</v>
@@ -3631,33 +3718,33 @@
         <v>996713</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s" s="0">
-        <v>125</v>
+        <v>254</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>115</v>
+        <v>241</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E7" s="0">
         <v>0</v>
@@ -3669,33 +3756,33 @@
         <v>996713</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s" s="0">
-        <v>126</v>
+        <v>255</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>119</v>
+        <v>223</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E8" s="0">
         <v>0</v>
@@ -3707,33 +3794,33 @@
         <v>996713</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="K8" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="J8" t="s" s="0">
-        <v>118</v>
-      </c>
-      <c r="K8" t="s" s="0">
-        <v>110</v>
-      </c>
       <c r="L8" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s" s="0">
-        <v>127</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E9" s="0">
         <v>0</v>
@@ -3745,19 +3832,19 @@
         <v>996713</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I9" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="K9" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="L9" t="s" s="0">
         <v>107</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>116</v>
-      </c>
-      <c r="K9" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="L9" t="s" s="0">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All tests for invoice validation for accounts for 1022 added
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0A763-D17A-492A-9AE7-F6CD672C8CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36271CF8-9850-4DA6-BEFC-1F050E635EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="TaxCode" sheetId="6" r:id="rId7"/>
     <sheet name="Reason" sheetId="7" r:id="rId8"/>
     <sheet name="POBasedInvoice" sheetId="8" r:id="rId9"/>
-    <sheet name="BADashboardPage" sheetId="9" r:id="rId10"/>
-    <sheet name="CommercialDashboardPage" sheetId="10" r:id="rId11"/>
-    <sheet name="BTBasedInvoice" sheetId="11" r:id="rId12"/>
+    <sheet name="InvoiceValidationAccounts_1022" sheetId="13" r:id="rId10"/>
+    <sheet name="BADashboardPage" sheetId="9" r:id="rId11"/>
+    <sheet name="CommercialDashboardPage" sheetId="10" r:id="rId12"/>
+    <sheet name="BTBasedInvoice" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -594,6 +595,41 @@
     <author>Nishant Gore</author>
   </authors>
   <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{11ABEAF0-579F-423C-9D30-ACA0A309C860}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+for search with invalid data test
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nishant Gore</author>
+  </authors>
+  <commentList>
     <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
@@ -623,7 +659,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="224">
   <si>
     <t>Medium</t>
   </si>
@@ -1171,18 +1207,6 @@
     <t>invalid_Baname</t>
   </si>
   <si>
-    <t>test_iqidek</t>
-  </si>
-  <si>
-    <t>test_ixhpgj</t>
-  </si>
-  <si>
-    <t>308645</t>
-  </si>
-  <si>
-    <t>726605</t>
-  </si>
-  <si>
     <t>Company Code</t>
   </si>
   <si>
@@ -1261,146 +1285,58 @@
     <t>testcode_xmwt</t>
   </si>
   <si>
-    <t>TESTINV45388</t>
-  </si>
-  <si>
-    <t>TESTINV02796</t>
-  </si>
-  <si>
-    <t>TESTINV41933</t>
-  </si>
-  <si>
-    <t>TESTINV76157</t>
-  </si>
-  <si>
-    <t>TESTINV49001</t>
-  </si>
-  <si>
-    <t>TESTINV45851</t>
-  </si>
-  <si>
-    <t>TESTINV13480</t>
-  </si>
-  <si>
-    <t>TESTINV62709</t>
-  </si>
-  <si>
-    <t>TESTINV78658</t>
-  </si>
-  <si>
-    <t>TESTINV88778</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>1.62</t>
-  </si>
-  <si>
-    <t>TESTINV43920</t>
-  </si>
-  <si>
-    <t>TESTINV76112</t>
-  </si>
-  <si>
-    <t>TESTINV06328</t>
-  </si>
-  <si>
-    <t>TESTINV80545</t>
-  </si>
-  <si>
-    <t>TESTINV97856</t>
-  </si>
-  <si>
-    <t>TESTINV60190</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>TESTINV05801</t>
-  </si>
-  <si>
-    <t>TESTINV16282</t>
-  </si>
-  <si>
-    <t>TESTINV26832</t>
-  </si>
-  <si>
-    <t>TESTINV64392</t>
-  </si>
-  <si>
-    <t>TESTINV32156</t>
-  </si>
-  <si>
-    <t>TESTINV95278</t>
-  </si>
-  <si>
-    <t>TESTINV08439</t>
-  </si>
-  <si>
-    <t>TESTINV92737</t>
-  </si>
-  <si>
-    <t>TESTINV88822</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>TESTINV92552</t>
-  </si>
-  <si>
-    <t>TESTINV77709</t>
-  </si>
-  <si>
-    <t>TESTINV34200</t>
-  </si>
-  <si>
-    <t>TESTINV43542</t>
-  </si>
-  <si>
-    <t>TESTINV45240</t>
-  </si>
-  <si>
-    <t>TESTINV42823</t>
-  </si>
-  <si>
-    <t>TESTINV84545</t>
-  </si>
-  <si>
-    <t>TESTINV64940</t>
-  </si>
-  <si>
-    <t>TESTINV02644</t>
-  </si>
-  <si>
-    <t>TESTINV03865</t>
-  </si>
-  <si>
-    <t>TESTINV39963</t>
-  </si>
-  <si>
-    <t>TESTINV48911</t>
-  </si>
-  <si>
-    <t>TESTINV71542</t>
-  </si>
-  <si>
-    <t>TESTINV17489</t>
-  </si>
-  <si>
-    <t>TESTINV19684</t>
+    <t>TESTINV54120</t>
+  </si>
+  <si>
+    <t>TESTINV57571</t>
+  </si>
+  <si>
+    <t>TESTINV22002</t>
+  </si>
+  <si>
+    <t>TESTINV74948</t>
+  </si>
+  <si>
+    <t>TESTINV16183</t>
+  </si>
+  <si>
+    <t>TESTINV98059</t>
+  </si>
+  <si>
+    <t>TESTINV96987</t>
+  </si>
+  <si>
+    <t>TESTINV73350</t>
+  </si>
+  <si>
+    <t>test_dbgwuz</t>
+  </si>
+  <si>
+    <t>test_mhvnnx</t>
+  </si>
+  <si>
+    <t>862781</t>
+  </si>
+  <si>
+    <t>935161</t>
+  </si>
+  <si>
+    <t>Commercial Name</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Bill Scan copy is not visible</t>
+  </si>
+  <si>
+    <t>Nasik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1872,10 +1808,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375"/>
-    <col min="2" max="2" customWidth="true" width="15.21875"/>
-    <col min="3" max="3" customWidth="true" width="15.109375"/>
-    <col min="4" max="4" customWidth="true" width="16.88671875"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1896,10 +1832,10 @@
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1910,27 +1846,27 @@
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>156</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1943,8 +1879,56 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49959C6-0CCE-4B10-9C08-2407A8BAC91A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -1952,15 +1936,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.21875"/>
-    <col min="2" max="2" customWidth="true" width="14.6640625"/>
-    <col min="3" max="3" customWidth="true" width="15.5546875"/>
-    <col min="4" max="4" customWidth="true" width="14.44140625"/>
-    <col min="5" max="5" customWidth="true" width="16.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="9" max="9" customWidth="true" width="16.33203125"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1993,88 +1977,88 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>115</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>106</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>1022</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>84</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>122</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>119</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>137</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>137</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>137</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>138</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>138</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>138</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>138</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>139</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>140</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>106</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>139</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>141</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>106</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2084,7 +2068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2094,43 +2078,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.88671875"/>
-    <col min="3" max="3" customWidth="true" width="11.88671875"/>
-    <col min="4" max="4" customWidth="true" width="17.44140625"/>
-    <col min="5" max="5" customWidth="true" width="21.77734375"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>123</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>124</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>125</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1022</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>128</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>106</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2140,7 +2124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -2150,10 +2134,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" customWidth="true" width="17.44140625"/>
-    <col min="12" max="12" customWidth="true" width="16.44140625"/>
-    <col min="13" max="13" customWidth="true" width="15.44140625"/>
-    <col min="14" max="14" customWidth="true" width="22.21875"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
+    <col min="14" max="14" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2201,354 +2185,354 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>142</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>144</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>996713</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>88</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>96</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>108</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>106</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>130</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>133</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>145</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>111</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>112</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>996713</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>89</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>97</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>108</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>106</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>130</v>
       </c>
-      <c r="M3" t="s" s="0">
+      <c r="M3" t="s">
         <v>135</v>
       </c>
-      <c r="N3" t="s" s="0">
+      <c r="N3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>146</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>113</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>114</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>996713</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>90</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>98</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>108</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K4" t="s">
         <v>106</v>
       </c>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>130</v>
       </c>
-      <c r="M4" t="s" s="0">
+      <c r="M4" t="s">
         <v>135</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>147</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>113</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>114</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>996713</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>91</v>
       </c>
-      <c r="I5" t="s" s="0">
+      <c r="I5" t="s">
         <v>99</v>
       </c>
-      <c r="J5" t="s" s="0">
+      <c r="J5" t="s">
         <v>113</v>
       </c>
-      <c r="K5" t="s" s="0">
+      <c r="K5" t="s">
         <v>106</v>
       </c>
-      <c r="L5" t="s" s="0">
+      <c r="L5" t="s">
         <v>130</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>136</v>
       </c>
-      <c r="N5" t="s" s="0">
+      <c r="N5" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>148</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>108</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>109</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>996713</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>92</v>
       </c>
-      <c r="I6" t="s" s="0">
+      <c r="I6" t="s">
         <v>100</v>
       </c>
-      <c r="J6" t="s" s="0">
+      <c r="J6" t="s">
         <v>111</v>
       </c>
-      <c r="K6" t="s" s="0">
+      <c r="K6" t="s">
         <v>106</v>
       </c>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>130</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>136</v>
       </c>
-      <c r="N6" t="s" s="0">
+      <c r="N6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>149</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>150</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>151</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>996713</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="H7" t="s">
         <v>93</v>
       </c>
-      <c r="I7" t="s" s="0">
+      <c r="I7" t="s">
         <v>101</v>
       </c>
-      <c r="J7" t="s" s="0">
+      <c r="J7" t="s">
         <v>110</v>
       </c>
-      <c r="K7" t="s" s="0">
+      <c r="K7" t="s">
         <v>106</v>
       </c>
-      <c r="L7" t="s" s="0">
+      <c r="L7" t="s">
         <v>130</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>136</v>
       </c>
-      <c r="N7" t="s" s="0">
+      <c r="N7" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>152</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>153</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>154</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>996713</v>
       </c>
-      <c r="H8" t="s" s="0">
+      <c r="H8" t="s">
         <v>94</v>
       </c>
-      <c r="I8" t="s" s="0">
+      <c r="I8" t="s">
         <v>102</v>
       </c>
-      <c r="J8" t="s" s="0">
+      <c r="J8" t="s">
         <v>113</v>
       </c>
-      <c r="K8" t="s" s="0">
+      <c r="K8" t="s">
         <v>106</v>
       </c>
-      <c r="L8" t="s" s="0">
+      <c r="L8" t="s">
         <v>130</v>
       </c>
-      <c r="M8" t="s" s="0">
+      <c r="M8" t="s">
         <v>133</v>
       </c>
-      <c r="N8" t="s" s="0">
+      <c r="N8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>155</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>150</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>151</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>996713</v>
       </c>
-      <c r="H9" t="s" s="0">
+      <c r="H9" t="s">
         <v>95</v>
       </c>
-      <c r="I9" t="s" s="0">
+      <c r="I9" t="s">
         <v>103</v>
       </c>
-      <c r="J9" t="s" s="0">
+      <c r="J9" t="s">
         <v>111</v>
       </c>
-      <c r="K9" t="s" s="0">
+      <c r="K9" t="s">
         <v>106</v>
       </c>
-      <c r="L9" t="s" s="0">
+      <c r="L9" t="s">
         <v>130</v>
       </c>
-      <c r="M9" t="s" s="0">
+      <c r="M9" t="s">
         <v>133</v>
       </c>
-      <c r="N9" t="s" s="0">
+      <c r="N9" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2567,16 +2551,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.77734375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.77734375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.77734375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.109375"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2621,217 +2605,217 @@
       <c r="C2" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>170</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>170</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>129</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
         <v>106</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>172</v>
       </c>
-      <c r="H3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J3" t="s" s="0">
+      <c r="H3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>122</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" t="s">
+        <v>171</v>
+      </c>
+      <c r="J4" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>129</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" t="s">
         <v>170</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>170</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J5" t="s" s="0">
+      <c r="F5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>173</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>174</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I6" t="s" s="0">
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" t="s">
         <v>175</v>
       </c>
-      <c r="J6" t="s" s="0">
+      <c r="J6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H7" t="s" s="0">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H7" t="s">
         <v>176</v>
       </c>
-      <c r="I7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J7" t="s" s="0">
+      <c r="I7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H8" t="s" s="0">
+      <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H8" t="s">
         <v>177</v>
       </c>
-      <c r="I8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J8" t="s" s="0">
+      <c r="I8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J8" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2839,63 +2823,63 @@
       <c r="A9" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>171</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" t="s">
+        <v>171</v>
+      </c>
+      <c r="J9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>171</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I10" t="s" s="0">
+      <c r="C10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" t="s">
+        <v>171</v>
+      </c>
+      <c r="G10" t="s">
+        <v>171</v>
+      </c>
+      <c r="H10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" t="s">
         <v>181</v>
       </c>
-      <c r="J10" t="s" s="0">
+      <c r="J10" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2907,7 +2891,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -2915,15 +2899,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.44140625"/>
-    <col min="4" max="4" customWidth="true" width="13.88671875"/>
-    <col min="5" max="5" customWidth="true" width="13.21875"/>
-    <col min="6" max="6" customWidth="true" width="17.77734375"/>
-    <col min="7" max="7" customWidth="true" width="13.88671875"/>
-    <col min="8" max="8" customWidth="true" width="12.0"/>
-    <col min="9" max="9" customWidth="true" width="23.5546875"/>
-    <col min="10" max="10" customWidth="true" width="20.44140625"/>
-    <col min="11" max="11" customWidth="true" width="26.33203125"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2963,12 +2947,12 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>182</v>
-      </c>
-      <c r="C2" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="B2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3">
@@ -2983,13 +2967,13 @@
       <c r="G2" s="3">
         <v>420</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="3">
@@ -3000,10 +2984,10 @@
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3">
@@ -3018,13 +3002,13 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="3">
@@ -3033,12 +3017,12 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>183</v>
-      </c>
-      <c r="C4" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="B4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3">
@@ -3053,13 +3037,13 @@
       <c r="G4" s="3">
         <v>420</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="3">
@@ -3083,7 +3067,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
@@ -3091,13 +3075,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.109375"/>
-    <col min="2" max="2" customWidth="true" width="12.33203125"/>
-    <col min="3" max="3" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" width="16.5546875"/>
-    <col min="5" max="5" customWidth="true" width="10.77734375"/>
-    <col min="6" max="7" customWidth="true" width="22.109375"/>
-    <col min="8" max="8" customWidth="true" width="12.21875"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3120,78 +3104,78 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" t="s">
         <v>186</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s" s="0">
-        <v>192</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>195</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>198</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>199</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s" s="0">
-        <v>193</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>196</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>200</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>201</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>190</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>191</v>
-      </c>
       <c r="G3" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>204</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>202</v>
-      </c>
-      <c r="E4" t="s" s="0">
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -3200,33 +3184,33 @@
       <c r="G4" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s" s="0">
-        <v>194</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>197</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>205</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>203</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3272,10 +3256,10 @@
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>159</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>160</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -3283,16 +3267,16 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>14</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3300,13 +3284,13 @@
       <c r="A4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3328,7 +3312,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.21875"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3340,18 +3324,18 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3370,9 +3354,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.44140625"/>
-    <col min="2" max="2" customWidth="true" width="16.0"/>
-    <col min="3" max="3" customWidth="true" width="14.21875"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3387,32 +3371,32 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s" s="0">
-        <v>206</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>207</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" t="s" s="0">
-        <v>208</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3432,8 +3416,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
-    <col min="2" max="2" customWidth="true" width="18.77734375"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3448,35 +3432,35 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s" s="0">
-        <v>211</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>209</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>210</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3489,20 +3473,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875"/>
-    <col min="4" max="4" customWidth="true" width="19.6640625"/>
-    <col min="7" max="7" customWidth="true" width="10.33203125"/>
-    <col min="8" max="8" customWidth="true" width="16.77734375"/>
-    <col min="9" max="9" customWidth="true" width="16.88671875"/>
-    <col min="11" max="11" customWidth="true" width="13.6640625"/>
-    <col min="12" max="12" customWidth="true" width="15.21875"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3544,306 +3528,306 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s" s="0">
-        <v>249</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>222</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>223</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>996713</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>88</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>96</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>222</v>
-      </c>
-      <c r="K2" t="s" s="0">
+      <c r="J2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K2" t="s">
         <v>106</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s" s="0">
-        <v>250</v>
-      </c>
-      <c r="B3" t="s" s="0">
+      <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
         <v>108</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>109</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>996713</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>89</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>97</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>108</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>106</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s" s="0">
-        <v>251</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>143</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>144</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="A4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>996713</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>90</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>98</v>
       </c>
-      <c r="J4" t="s" s="0">
-        <v>143</v>
-      </c>
-      <c r="K4" t="s" s="0">
+      <c r="J4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K4" t="s">
         <v>106</v>
       </c>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s" s="0">
-        <v>252</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="A5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>996713</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>91</v>
       </c>
-      <c r="I5" t="s" s="0">
+      <c r="I5" t="s">
         <v>99</v>
       </c>
-      <c r="J5" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="K5" t="s" s="0">
+      <c r="J5" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" t="s">
         <v>106</v>
       </c>
-      <c r="L5" t="s" s="0">
+      <c r="L5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>150</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>151</v>
-      </c>
-      <c r="D6" t="s" s="0">
+      <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>996713</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>92</v>
       </c>
-      <c r="I6" t="s" s="0">
+      <c r="I6" t="s">
         <v>100</v>
       </c>
-      <c r="J6" t="s" s="0">
-        <v>150</v>
-      </c>
-      <c r="K6" t="s" s="0">
+      <c r="J6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6" t="s">
         <v>106</v>
       </c>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>241</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>996713</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="H7" t="s">
         <v>93</v>
       </c>
-      <c r="I7" t="s" s="0">
+      <c r="I7" t="s">
         <v>101</v>
       </c>
-      <c r="J7" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="K7" t="s" s="0">
+      <c r="J7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" t="s">
         <v>106</v>
       </c>
-      <c r="L7" t="s" s="0">
+      <c r="L7" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" t="s" s="0">
-        <v>255</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>222</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>223</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>996713</v>
       </c>
-      <c r="H8" t="s" s="0">
+      <c r="H8" t="s">
         <v>94</v>
       </c>
-      <c r="I8" t="s" s="0">
+      <c r="I8" t="s">
         <v>102</v>
       </c>
-      <c r="J8" t="s" s="0">
-        <v>222</v>
-      </c>
-      <c r="K8" t="s" s="0">
+      <c r="J8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K8" t="s">
         <v>106</v>
       </c>
-      <c r="L8" t="s" s="0">
+      <c r="L8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" t="s" s="0">
-        <v>256</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>153</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>154</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="A9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>996713</v>
       </c>
-      <c r="H9" t="s" s="0">
+      <c r="H9" t="s">
         <v>95</v>
       </c>
-      <c r="I9" t="s" s="0">
+      <c r="I9" t="s">
         <v>103</v>
       </c>
-      <c r="J9" t="s" s="0">
-        <v>153</v>
-      </c>
-      <c r="K9" t="s" s="0">
+      <c r="J9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" t="s">
         <v>106</v>
       </c>
-      <c r="L9" t="s" s="0">
+      <c r="L9" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extra wait for loader added in user, ba, customer and withholding page
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
@@ -29,7 +29,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -659,7 +659,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="263">
   <si>
     <t>Medium</t>
   </si>
@@ -1331,12 +1331,130 @@
   </si>
   <si>
     <t>Nasik</t>
+  </si>
+  <si>
+    <t>test_zhubbb</t>
+  </si>
+  <si>
+    <t>test_optofy</t>
+  </si>
+  <si>
+    <t>156489</t>
+  </si>
+  <si>
+    <t>026793</t>
+  </si>
+  <si>
+    <t>test_wgmael</t>
+  </si>
+  <si>
+    <t>test_wbddxq</t>
+  </si>
+  <si>
+    <t>577214</t>
+  </si>
+  <si>
+    <t>053263</t>
+  </si>
+  <si>
+    <t>test_tcqbsw</t>
+  </si>
+  <si>
+    <t>test_pwuzrr</t>
+  </si>
+  <si>
+    <t>013052</t>
+  </si>
+  <si>
+    <t>360040</t>
+  </si>
+  <si>
+    <t>test_acrxtu</t>
+  </si>
+  <si>
+    <t>test_upzbwk</t>
+  </si>
+  <si>
+    <t>366055</t>
+  </si>
+  <si>
+    <t>598395</t>
+  </si>
+  <si>
+    <t>355338</t>
+  </si>
+  <si>
+    <t>795881</t>
+  </si>
+  <si>
+    <t>350600</t>
+  </si>
+  <si>
+    <t>508161</t>
+  </si>
+  <si>
+    <t>183514</t>
+  </si>
+  <si>
+    <t>test_ytwfqd</t>
+  </si>
+  <si>
+    <t>test_bfcgbm</t>
+  </si>
+  <si>
+    <t>551123</t>
+  </si>
+  <si>
+    <t>982240</t>
+  </si>
+  <si>
+    <t>test_tnmert</t>
+  </si>
+  <si>
+    <t>test_wwbbfx</t>
+  </si>
+  <si>
+    <t>391945</t>
+  </si>
+  <si>
+    <t>467289</t>
+  </si>
+  <si>
+    <t>test_cohivg</t>
+  </si>
+  <si>
+    <t>test_xahvnh</t>
+  </si>
+  <si>
+    <t>test_ysamox</t>
+  </si>
+  <si>
+    <t>test_afhozv</t>
+  </si>
+  <si>
+    <t>test_dcoyki</t>
+  </si>
+  <si>
+    <t>087995</t>
+  </si>
+  <si>
+    <t>654812</t>
+  </si>
+  <si>
+    <t>137331</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>37</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1808,10 +1926,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375"/>
+    <col min="2" max="2" customWidth="true" width="15.21875"/>
+    <col min="3" max="3" customWidth="true" width="15.109375"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1830,12 +1948,12 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2">
+        <v>253</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>251</v>
+      </c>
+      <c r="C2" s="0">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1846,27 +1964,27 @@
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4">
+      <c r="A4" t="s" s="0">
+        <v>254</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="C4" s="0">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>54</v>
       </c>
     </row>
@@ -1888,9 +2006,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0"/>
+    <col min="2" max="2" customWidth="true" width="18.0"/>
+    <col min="3" max="3" customWidth="true" width="23.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1905,18 +2023,18 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>106</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -1928,7 +2046,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -1936,15 +2054,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="29.21875"/>
+    <col min="2" max="2" customWidth="true" width="14.6640625"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875"/>
+    <col min="4" max="4" customWidth="true" width="14.44140625"/>
+    <col min="5" max="5" customWidth="true" width="16.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="9" max="9" customWidth="true" width="16.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1977,88 +2095,88 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1022</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>130</v>
       </c>
     </row>
@@ -2078,43 +2196,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.88671875"/>
+    <col min="3" max="3" customWidth="true" width="11.88671875"/>
+    <col min="4" max="4" customWidth="true" width="17.44140625"/>
+    <col min="5" max="5" customWidth="true" width="21.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>126</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1022</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>106</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>129</v>
       </c>
     </row>
@@ -2134,10 +2252,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" customWidth="1"/>
-    <col min="14" max="14" width="22.21875" customWidth="1"/>
+    <col min="11" max="11" customWidth="true" width="17.44140625"/>
+    <col min="12" max="12" customWidth="true" width="16.44140625"/>
+    <col min="13" max="13" customWidth="true" width="15.44140625"/>
+    <col min="14" max="14" customWidth="true" width="22.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2185,354 +2303,354 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>996713</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>996713</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>996713</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>996713</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>996713</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>996713</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>996713</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" t="s" s="0">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>996713</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" t="s" s="0">
         <v>134</v>
       </c>
     </row>
@@ -2551,16 +2669,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2605,217 +2723,217 @@
       <c r="C2" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="F2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" t="s">
-        <v>171</v>
-      </c>
-      <c r="I2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="F2" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="J2" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="B3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>172</v>
       </c>
-      <c r="H3" t="s">
-        <v>171</v>
-      </c>
-      <c r="I3" t="s">
-        <v>171</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="H3" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="J3" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" t="s">
-        <v>171</v>
-      </c>
-      <c r="I4" t="s">
-        <v>171</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="J4" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="B5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="F5" t="s">
-        <v>171</v>
-      </c>
-      <c r="G5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I5" t="s">
-        <v>171</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="F5" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="J5" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>173</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="C6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" t="s">
-        <v>171</v>
-      </c>
-      <c r="G6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H6" t="s">
-        <v>171</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="C6" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="I6" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" t="s">
-        <v>171</v>
-      </c>
-      <c r="G7" t="s">
-        <v>171</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="A7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="I7" t="s">
-        <v>171</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="J7" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C8" t="s">
-        <v>171</v>
-      </c>
-      <c r="D8" t="s">
-        <v>171</v>
-      </c>
-      <c r="E8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F8" t="s">
-        <v>171</v>
-      </c>
-      <c r="G8" t="s">
-        <v>171</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="A8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H8" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="I8" t="s">
-        <v>171</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="J8" t="s" s="0">
         <v>171</v>
       </c>
     </row>
@@ -2823,63 +2941,63 @@
       <c r="A9" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>171</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="D9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G9" t="s">
-        <v>171</v>
-      </c>
-      <c r="H9" t="s">
-        <v>171</v>
-      </c>
-      <c r="I9" t="s">
-        <v>171</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="D9" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="J9" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>171</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D10" t="s">
-        <v>171</v>
-      </c>
-      <c r="E10" t="s">
-        <v>171</v>
-      </c>
-      <c r="F10" t="s">
-        <v>171</v>
-      </c>
-      <c r="G10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H10" t="s">
-        <v>171</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="C10" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="I10" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>171</v>
       </c>
     </row>
@@ -2891,7 +3009,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -2899,15 +3017,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="13.44140625"/>
+    <col min="4" max="4" customWidth="true" width="13.88671875"/>
+    <col min="5" max="5" customWidth="true" width="13.21875"/>
+    <col min="6" max="6" customWidth="true" width="17.77734375"/>
+    <col min="7" max="7" customWidth="true" width="13.88671875"/>
+    <col min="8" max="8" customWidth="true" width="12.0"/>
+    <col min="9" max="9" customWidth="true" width="23.5546875"/>
+    <col min="10" max="10" customWidth="true" width="20.44140625"/>
+    <col min="11" max="11" customWidth="true" width="26.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2947,12 +3065,12 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
       <c r="D2" s="3">
@@ -2967,13 +3085,13 @@
       <c r="G2" s="3">
         <v>420</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>3</v>
       </c>
       <c r="K2" s="3">
@@ -2984,10 +3102,10 @@
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>5</v>
       </c>
       <c r="D3" s="3">
@@ -3002,13 +3120,13 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>3</v>
       </c>
       <c r="K3" s="3">
@@ -3017,12 +3135,12 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>237</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D4" s="3">
@@ -3037,13 +3155,13 @@
       <c r="G4" s="3">
         <v>420</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K4" s="3">
@@ -3067,7 +3185,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
@@ -3075,13 +3193,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="7" width="22.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.109375"/>
+    <col min="2" max="2" customWidth="true" width="12.33203125"/>
+    <col min="3" max="3" customWidth="true" width="16.0"/>
+    <col min="4" max="4" customWidth="true" width="16.5546875"/>
+    <col min="5" max="5" customWidth="true" width="10.77734375"/>
+    <col min="6" max="7" customWidth="true" width="22.109375"/>
+    <col min="8" max="8" customWidth="true" width="12.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3111,19 +3229,19 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>195</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -3132,24 +3250,24 @@
       <c r="G2" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" t="s" s="0">
+        <v>256</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>186</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -3158,24 +3276,24 @@
       <c r="G3" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -3184,24 +3302,24 @@
       <c r="G4" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>201</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -3210,7 +3328,7 @@
       <c r="G5" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>171</v>
       </c>
     </row>
@@ -3256,27 +3374,27 @@
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" t="s">
-        <v>160</v>
+      <c r="B2" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>262</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>48</v>
       </c>
     </row>
@@ -3284,13 +3402,13 @@
       <c r="A4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>60</v>
       </c>
     </row>
@@ -3312,7 +3430,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3324,18 +3442,18 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>69</v>
       </c>
     </row>
@@ -3354,9 +3472,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.44140625"/>
+    <col min="2" max="2" customWidth="true" width="16.0"/>
+    <col min="3" max="3" customWidth="true" width="14.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3371,32 +3489,32 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>39</v>
       </c>
     </row>
@@ -3416,8 +3534,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
+    <col min="2" max="2" customWidth="true" width="18.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3432,35 +3550,35 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>48</v>
       </c>
     </row>
@@ -3479,14 +3597,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875"/>
+    <col min="4" max="4" customWidth="true" width="19.6640625"/>
+    <col min="7" max="7" customWidth="true" width="10.33203125"/>
+    <col min="8" max="8" customWidth="true" width="16.77734375"/>
+    <col min="9" max="9" customWidth="true" width="16.88671875"/>
+    <col min="11" max="11" customWidth="true" width="13.6640625"/>
+    <col min="12" max="12" customWidth="true" width="15.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3528,306 +3646,306 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>996713</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>209</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>996713</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>210</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>996713</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>996713</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>996713</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>996713</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>996713</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>215</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>996713</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>107</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes made in ba, user, customer and withholding page
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -659,7 +659,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="338">
   <si>
     <t>Medium</t>
   </si>
@@ -1448,6 +1448,231 @@
   </si>
   <si>
     <t>37</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>292133</t>
+  </si>
+  <si>
+    <t>356910</t>
+  </si>
+  <si>
+    <t>test_jrbzsu</t>
+  </si>
+  <si>
+    <t>test_lriond</t>
+  </si>
+  <si>
+    <t>426373</t>
+  </si>
+  <si>
+    <t>246715</t>
+  </si>
+  <si>
+    <t>test_alvsex</t>
+  </si>
+  <si>
+    <t>test_xribzl</t>
+  </si>
+  <si>
+    <t>652171</t>
+  </si>
+  <si>
+    <t>437339</t>
+  </si>
+  <si>
+    <t>test_cntilp</t>
+  </si>
+  <si>
+    <t>test_ljkjho</t>
+  </si>
+  <si>
+    <t>219118</t>
+  </si>
+  <si>
+    <t>918886</t>
+  </si>
+  <si>
+    <t>test_pndubh</t>
+  </si>
+  <si>
+    <t>test_ulqlhd</t>
+  </si>
+  <si>
+    <t>test_fqthyu</t>
+  </si>
+  <si>
+    <t>test_mzktfs</t>
+  </si>
+  <si>
+    <t>825516</t>
+  </si>
+  <si>
+    <t>test_apkpsa</t>
+  </si>
+  <si>
+    <t>test_pbepeh</t>
+  </si>
+  <si>
+    <t>500059</t>
+  </si>
+  <si>
+    <t>836500</t>
+  </si>
+  <si>
+    <t>215506</t>
+  </si>
+  <si>
+    <t>test_kyrphj</t>
+  </si>
+  <si>
+    <t>test_hbkzok</t>
+  </si>
+  <si>
+    <t>096215</t>
+  </si>
+  <si>
+    <t>108551</t>
+  </si>
+  <si>
+    <t>test_razaxr</t>
+  </si>
+  <si>
+    <t>test_ccnlpz</t>
+  </si>
+  <si>
+    <t>728040</t>
+  </si>
+  <si>
+    <t>643928</t>
+  </si>
+  <si>
+    <t>test_ncgnum</t>
+  </si>
+  <si>
+    <t>test_xlhqit</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>test_llglgf</t>
+  </si>
+  <si>
+    <t>test_tmndby</t>
+  </si>
+  <si>
+    <t>200149</t>
+  </si>
+  <si>
+    <t>test_qqwaie</t>
+  </si>
+  <si>
+    <t>test_rljdvy</t>
+  </si>
+  <si>
+    <t>518544</t>
+  </si>
+  <si>
+    <t>test_wdgcjn</t>
+  </si>
+  <si>
+    <t>test_wpuste</t>
+  </si>
+  <si>
+    <t>146307</t>
+  </si>
+  <si>
+    <t>test_vhppwh</t>
+  </si>
+  <si>
+    <t>test_vqxyyk</t>
+  </si>
+  <si>
+    <t>test_oipajf</t>
+  </si>
+  <si>
+    <t>896213</t>
+  </si>
+  <si>
+    <t>624880</t>
+  </si>
+  <si>
+    <t>710338</t>
+  </si>
+  <si>
+    <t>test_nmlnbr</t>
+  </si>
+  <si>
+    <t>test_qfdtbo</t>
+  </si>
+  <si>
+    <t>094437</t>
+  </si>
+  <si>
+    <t>test_nsxsfc</t>
+  </si>
+  <si>
+    <t>test_udfgir</t>
+  </si>
+  <si>
+    <t>205028</t>
+  </si>
+  <si>
+    <t>test_mphoyo</t>
+  </si>
+  <si>
+    <t>test_oovgak</t>
+  </si>
+  <si>
+    <t>760604</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>545960</t>
+  </si>
+  <si>
+    <t>820723</t>
+  </si>
+  <si>
+    <t>test_brptge</t>
+  </si>
+  <si>
+    <t>test_ceetfd</t>
+  </si>
+  <si>
+    <t>test_zpoyjz</t>
+  </si>
+  <si>
+    <t>test_kvauhi</t>
+  </si>
+  <si>
+    <t>test_wlmvuo</t>
+  </si>
+  <si>
+    <t>634223</t>
+  </si>
+  <si>
+    <t>261002</t>
+  </si>
+  <si>
+    <t>062637</t>
   </si>
 </sst>
 </file>
@@ -1948,10 +2173,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>253</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>251</v>
+        <v>328</v>
       </c>
       <c r="C2" s="0">
         <v>14</v>
@@ -1976,10 +2201,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s" s="0">
-        <v>254</v>
+        <v>331</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>252</v>
+        <v>329</v>
       </c>
       <c r="C4" s="0">
         <v>12</v>
@@ -3065,10 +3290,10 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>238</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>5</v>
@@ -3135,10 +3360,10 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>238</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>237</v>
+        <v>322</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>6</v>
@@ -3230,10 +3455,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s" s="0">
-        <v>255</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>258</v>
+        <v>335</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>194</v>
@@ -3256,10 +3481,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s" s="0">
-        <v>256</v>
+        <v>333</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>259</v>
+        <v>336</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>196</v>
@@ -3308,10 +3533,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s" s="0">
-        <v>257</v>
+        <v>334</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>260</v>
+        <v>337</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>201</v>
@@ -3375,10 +3600,10 @@
         <v>59</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>261</v>
+        <v>326</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>262</v>
+        <v>327</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
All tests for accounts and taxation for all companies added
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36271CF8-9850-4DA6-BEFC-1F050E635EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291A58F8-8CCF-4B08-88AD-D46717BE3F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,15 @@
     <sheet name="Reason" sheetId="7" r:id="rId8"/>
     <sheet name="POBasedInvoice" sheetId="8" r:id="rId9"/>
     <sheet name="InvoiceValidationAccounts_1022" sheetId="13" r:id="rId10"/>
-    <sheet name="BADashboardPage" sheetId="9" r:id="rId11"/>
-    <sheet name="CommercialDashboardPage" sheetId="10" r:id="rId12"/>
-    <sheet name="BTBasedInvoice" sheetId="11" r:id="rId13"/>
+    <sheet name="InvoiceValidationAccounts_MERU" sheetId="14" r:id="rId11"/>
+    <sheet name="InvoiceValidationAccounts_MESPL" sheetId="15" r:id="rId12"/>
+    <sheet name="BADashboardPage" sheetId="9" r:id="rId13"/>
+    <sheet name="CommercialDashboardPage" sheetId="10" r:id="rId14"/>
+    <sheet name="BTBasedInvoice" sheetId="11" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -630,6 +632,76 @@
     <author>Nishant Gore</author>
   </authors>
   <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{372686DC-7F29-484B-AA8C-7F608A0DCE09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+for search with invalid data test
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nishant Gore</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{19C677AE-A9AD-45B9-9AA5-E1B1599C55C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nishant Gore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+for search with invalid data test
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nishant Gore</author>
+  </authors>
+  <commentList>
     <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
@@ -659,7 +731,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="224">
   <si>
     <t>Medium</t>
   </si>
@@ -820,9 +892,6 @@
     <t>customer_drop</t>
   </si>
   <si>
-    <t>Akash</t>
-  </si>
-  <si>
     <t>AOB</t>
   </si>
   <si>
@@ -1129,21 +1198,6 @@
     <t>TESTINV9890</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>594194</t>
-  </si>
-  <si>
-    <t>616938</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>Reject reason</t>
   </si>
   <si>
@@ -1225,24 +1279,6 @@
     <t>testemail@gmail.com</t>
   </si>
   <si>
-    <t>test_kmrahi</t>
-  </si>
-  <si>
-    <t>test_cnthne</t>
-  </si>
-  <si>
-    <t>test_odxlxy</t>
-  </si>
-  <si>
-    <t>851517</t>
-  </si>
-  <si>
-    <t>382474</t>
-  </si>
-  <si>
-    <t>214129</t>
-  </si>
-  <si>
     <t>test_first_name_1</t>
   </si>
   <si>
@@ -1309,18 +1345,6 @@
     <t>TESTINV73350</t>
   </si>
   <si>
-    <t>test_dbgwuz</t>
-  </si>
-  <si>
-    <t>test_mhvnnx</t>
-  </si>
-  <si>
-    <t>862781</t>
-  </si>
-  <si>
-    <t>935161</t>
-  </si>
-  <si>
     <t>Commercial Name</t>
   </si>
   <si>
@@ -1333,297 +1357,6 @@
     <t>Nasik</t>
   </si>
   <si>
-    <t>test_zhubbb</t>
-  </si>
-  <si>
-    <t>test_optofy</t>
-  </si>
-  <si>
-    <t>156489</t>
-  </si>
-  <si>
-    <t>026793</t>
-  </si>
-  <si>
-    <t>test_wgmael</t>
-  </si>
-  <si>
-    <t>test_wbddxq</t>
-  </si>
-  <si>
-    <t>577214</t>
-  </si>
-  <si>
-    <t>053263</t>
-  </si>
-  <si>
-    <t>test_tcqbsw</t>
-  </si>
-  <si>
-    <t>test_pwuzrr</t>
-  </si>
-  <si>
-    <t>013052</t>
-  </si>
-  <si>
-    <t>360040</t>
-  </si>
-  <si>
-    <t>test_acrxtu</t>
-  </si>
-  <si>
-    <t>test_upzbwk</t>
-  </si>
-  <si>
-    <t>366055</t>
-  </si>
-  <si>
-    <t>598395</t>
-  </si>
-  <si>
-    <t>355338</t>
-  </si>
-  <si>
-    <t>795881</t>
-  </si>
-  <si>
-    <t>350600</t>
-  </si>
-  <si>
-    <t>508161</t>
-  </si>
-  <si>
-    <t>183514</t>
-  </si>
-  <si>
-    <t>test_ytwfqd</t>
-  </si>
-  <si>
-    <t>test_bfcgbm</t>
-  </si>
-  <si>
-    <t>551123</t>
-  </si>
-  <si>
-    <t>982240</t>
-  </si>
-  <si>
-    <t>test_tnmert</t>
-  </si>
-  <si>
-    <t>test_wwbbfx</t>
-  </si>
-  <si>
-    <t>391945</t>
-  </si>
-  <si>
-    <t>467289</t>
-  </si>
-  <si>
-    <t>test_cohivg</t>
-  </si>
-  <si>
-    <t>test_xahvnh</t>
-  </si>
-  <si>
-    <t>test_ysamox</t>
-  </si>
-  <si>
-    <t>test_afhozv</t>
-  </si>
-  <si>
-    <t>test_dcoyki</t>
-  </si>
-  <si>
-    <t>087995</t>
-  </si>
-  <si>
-    <t>654812</t>
-  </si>
-  <si>
-    <t>137331</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>292133</t>
-  </si>
-  <si>
-    <t>356910</t>
-  </si>
-  <si>
-    <t>test_jrbzsu</t>
-  </si>
-  <si>
-    <t>test_lriond</t>
-  </si>
-  <si>
-    <t>426373</t>
-  </si>
-  <si>
-    <t>246715</t>
-  </si>
-  <si>
-    <t>test_alvsex</t>
-  </si>
-  <si>
-    <t>test_xribzl</t>
-  </si>
-  <si>
-    <t>652171</t>
-  </si>
-  <si>
-    <t>437339</t>
-  </si>
-  <si>
-    <t>test_cntilp</t>
-  </si>
-  <si>
-    <t>test_ljkjho</t>
-  </si>
-  <si>
-    <t>219118</t>
-  </si>
-  <si>
-    <t>918886</t>
-  </si>
-  <si>
-    <t>test_pndubh</t>
-  </si>
-  <si>
-    <t>test_ulqlhd</t>
-  </si>
-  <si>
-    <t>test_fqthyu</t>
-  </si>
-  <si>
-    <t>test_mzktfs</t>
-  </si>
-  <si>
-    <t>825516</t>
-  </si>
-  <si>
-    <t>test_apkpsa</t>
-  </si>
-  <si>
-    <t>test_pbepeh</t>
-  </si>
-  <si>
-    <t>500059</t>
-  </si>
-  <si>
-    <t>836500</t>
-  </si>
-  <si>
-    <t>215506</t>
-  </si>
-  <si>
-    <t>test_kyrphj</t>
-  </si>
-  <si>
-    <t>test_hbkzok</t>
-  </si>
-  <si>
-    <t>096215</t>
-  </si>
-  <si>
-    <t>108551</t>
-  </si>
-  <si>
-    <t>test_razaxr</t>
-  </si>
-  <si>
-    <t>test_ccnlpz</t>
-  </si>
-  <si>
-    <t>728040</t>
-  </si>
-  <si>
-    <t>643928</t>
-  </si>
-  <si>
-    <t>test_ncgnum</t>
-  </si>
-  <si>
-    <t>test_xlhqit</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>test_llglgf</t>
-  </si>
-  <si>
-    <t>test_tmndby</t>
-  </si>
-  <si>
-    <t>200149</t>
-  </si>
-  <si>
-    <t>test_qqwaie</t>
-  </si>
-  <si>
-    <t>test_rljdvy</t>
-  </si>
-  <si>
-    <t>518544</t>
-  </si>
-  <si>
-    <t>test_wdgcjn</t>
-  </si>
-  <si>
-    <t>test_wpuste</t>
-  </si>
-  <si>
-    <t>146307</t>
-  </si>
-  <si>
-    <t>test_vhppwh</t>
-  </si>
-  <si>
-    <t>test_vqxyyk</t>
-  </si>
-  <si>
-    <t>test_oipajf</t>
-  </si>
-  <si>
-    <t>896213</t>
-  </si>
-  <si>
-    <t>624880</t>
-  </si>
-  <si>
-    <t>710338</t>
-  </si>
-  <si>
-    <t>test_nmlnbr</t>
-  </si>
-  <si>
-    <t>test_qfdtbo</t>
-  </si>
-  <si>
-    <t>094437</t>
-  </si>
-  <si>
-    <t>test_nsxsfc</t>
-  </si>
-  <si>
-    <t>test_udfgir</t>
-  </si>
-  <si>
-    <t>205028</t>
-  </si>
-  <si>
     <t>test_mphoyo</t>
   </si>
   <si>
@@ -1633,12 +1366,6 @@
     <t>760604</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
     <t>81</t>
   </si>
   <si>
@@ -1673,13 +1400,15 @@
   </si>
   <si>
     <t>062637</t>
+  </si>
+  <si>
+    <t>Anusha Palle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -2151,10 +1880,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375"/>
-    <col min="2" max="2" customWidth="true" width="15.21875"/>
-    <col min="3" max="3" customWidth="true" width="15.109375"/>
-    <col min="4" max="4" customWidth="true" width="16.88671875"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2173,44 +1902,44 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>328</v>
-      </c>
-      <c r="C2" s="0">
+        <v>215</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>54</v>
+      <c r="D3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s" s="0">
-        <v>331</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>329</v>
-      </c>
-      <c r="C4" s="0">
+      <c r="A4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>54</v>
+      <c r="D4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2225,42 +1954,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49959C6-0CCE-4B10-9C08-2407A8BAC91A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.0"/>
-    <col min="2" max="2" customWidth="true" width="18.0"/>
-    <col min="3" max="3" customWidth="true" width="23.77734375"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>222</v>
+      <c r="C2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s" s="0">
-        <v>223</v>
+      <c r="A3" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2270,8 +1999,104 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CA415D-4F09-4A01-BE37-97DA44017A31}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8206F6E4-0F0D-4202-8599-954FFEEC985A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -2279,130 +2104,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.21875"/>
-    <col min="2" max="2" customWidth="true" width="14.6640625"/>
-    <col min="3" max="3" customWidth="true" width="15.5546875"/>
-    <col min="4" max="4" customWidth="true" width="14.44140625"/>
-    <col min="5" max="5" customWidth="true" width="16.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="9" max="9" customWidth="true" width="16.33203125"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2">
+        <v>1022</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s" s="0">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>115</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="E2" s="0">
-        <v>1022</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>119</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>121</v>
-      </c>
-    </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
         <v>137</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="F3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="G3" t="s">
         <v>137</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="H3" t="s">
         <v>137</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="I3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
         <v>138</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
         <v>138</v>
       </c>
-      <c r="G3" t="s" s="0">
-        <v>138</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>138</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s" s="0">
-        <v>139</v>
-      </c>
-      <c r="B4" t="s" s="0">
+      <c r="B5" t="s">
         <v>140</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s" s="0">
-        <v>139</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>141</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>130</v>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +2236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2421,44 +2246,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.88671875"/>
-    <col min="3" max="3" customWidth="true" width="11.88671875"/>
-    <col min="4" max="4" customWidth="true" width="17.44140625"/>
-    <col min="5" max="5" customWidth="true" width="21.77734375"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
         <v>123</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" t="s">
         <v>124</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="D1" t="s">
         <v>125</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="E1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" t="s" s="0">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1022</v>
+      </c>
+      <c r="B2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="0">
-        <v>1022</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
         <v>128</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2467,7 +2292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -2477,406 +2302,406 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" customWidth="true" width="17.44140625"/>
-    <col min="12" max="12" customWidth="true" width="16.44140625"/>
-    <col min="13" max="13" customWidth="true" width="15.44140625"/>
-    <col min="14" max="14" customWidth="true" width="22.21875"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
+    <col min="14" max="14" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>996713</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="L2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>143</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="N2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
         <v>144</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E2" s="0">
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G3">
         <v>996713</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I3" t="s">
         <v>96</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>996713</v>
+      </c>
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" t="s">
+        <v>134</v>
+      </c>
+      <c r="N4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>996713</v>
+      </c>
+      <c r="H5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K5" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M5" t="s">
+        <v>135</v>
+      </c>
+      <c r="N5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
         <v>108</v>
       </c>
-      <c r="K2" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M2" t="s" s="0">
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>996713</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" t="s">
+        <v>129</v>
+      </c>
+      <c r="M6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N6" t="s">
         <v>133</v>
       </c>
-      <c r="N2" t="s" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s" s="0">
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>996713</v>
+      </c>
+      <c r="H7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" t="s">
+        <v>135</v>
+      </c>
+      <c r="N7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>996713</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" t="s">
         <v>112</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E3" s="0">
+      <c r="K8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" t="s">
+        <v>129</v>
+      </c>
+      <c r="M8" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G9">
         <v>996713</v>
       </c>
-      <c r="H3" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L3" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M3" t="s" s="0">
-        <v>135</v>
-      </c>
-      <c r="N3" t="s" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s" s="0">
-        <v>146</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>114</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E4" s="0">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>90</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>98</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L4" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M4" t="s" s="0">
-        <v>135</v>
-      </c>
-      <c r="N4" t="s" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s" s="0">
-        <v>147</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E5" s="0">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="K5" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L5" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M5" t="s" s="0">
-        <v>136</v>
-      </c>
-      <c r="N5" t="s" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s" s="0">
-        <v>148</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E6" s="0">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="K6" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>136</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s" s="0">
-        <v>149</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>150</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>151</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E7" s="0">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="J7" t="s" s="0">
+      <c r="H9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" t="s">
         <v>110</v>
       </c>
-      <c r="K7" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M7" t="s" s="0">
-        <v>136</v>
-      </c>
-      <c r="N7" t="s" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s" s="0">
-        <v>152</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>153</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>154</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E8" s="0">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>102</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="K8" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L8" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M8" t="s" s="0">
+      <c r="K9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" t="s">
+        <v>129</v>
+      </c>
+      <c r="M9" t="s">
+        <v>132</v>
+      </c>
+      <c r="N9" t="s">
         <v>133</v>
-      </c>
-      <c r="N8" t="s" s="0">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s" s="0">
-        <v>155</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>150</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>151</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E9" s="0">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>103</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="K9" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L9" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="M9" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="N9" t="s" s="0">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2894,336 +2719,336 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.77734375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.77734375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.77734375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.109375"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" t="s">
+        <v>165</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B6" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H6" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" t="s">
         <v>169</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="J6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" t="s">
         <v>170</v>
       </c>
-      <c r="E2" t="s" s="0">
-        <v>170</v>
-      </c>
-      <c r="F2" t="s" s="0">
+      <c r="I7" t="s">
+        <v>165</v>
+      </c>
+      <c r="J7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" t="s">
         <v>171</v>
       </c>
-      <c r="G2" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s" s="0">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>172</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s" s="0">
-        <v>129</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>170</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>170</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s" s="0">
-        <v>173</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>174</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>175</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>176</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>177</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>171</v>
+      <c r="I8" t="s">
+        <v>165</v>
+      </c>
+      <c r="J8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H9" t="s">
+        <v>165</v>
+      </c>
+      <c r="I9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J9" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s" s="0">
-        <v>171</v>
+      <c r="A10" t="s">
+        <v>165</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I10" t="s" s="0">
-        <v>181</v>
-      </c>
-      <c r="J10" t="s" s="0">
-        <v>171</v>
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3234,7 +3059,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -3242,15 +3067,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.44140625"/>
-    <col min="4" max="4" customWidth="true" width="13.88671875"/>
-    <col min="5" max="5" customWidth="true" width="13.21875"/>
-    <col min="6" max="6" customWidth="true" width="17.77734375"/>
-    <col min="7" max="7" customWidth="true" width="13.88671875"/>
-    <col min="8" max="8" customWidth="true" width="12.0"/>
-    <col min="9" max="9" customWidth="true" width="23.5546875"/>
-    <col min="10" max="10" customWidth="true" width="20.44140625"/>
-    <col min="11" max="11" customWidth="true" width="26.33203125"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3290,12 +3115,12 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>321</v>
-      </c>
-      <c r="C2" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3">
@@ -3310,13 +3135,13 @@
       <c r="G2" s="3">
         <v>420</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="3">
@@ -3327,10 +3152,10 @@
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3">
@@ -3345,13 +3170,13 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="3">
@@ -3360,12 +3185,12 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>322</v>
-      </c>
-      <c r="C4" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3">
@@ -3380,13 +3205,13 @@
       <c r="G4" s="3">
         <v>420</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="3">
@@ -3410,7 +3235,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
@@ -3418,13 +3243,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.109375"/>
-    <col min="2" max="2" customWidth="true" width="12.33203125"/>
-    <col min="3" max="3" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" width="16.5546875"/>
-    <col min="5" max="5" customWidth="true" width="10.77734375"/>
-    <col min="6" max="7" customWidth="true" width="22.109375"/>
-    <col min="8" max="8" customWidth="true" width="12.21875"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3447,114 +3272,114 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s" s="0">
-        <v>332</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>194</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>195</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" t="s">
         <v>184</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="D3" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s" s="0">
-        <v>333</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>336</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>196</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>197</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>186</v>
+      <c r="E3" t="s">
+        <v>180</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>171</v>
+        <v>165</v>
+      </c>
+      <c r="H3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>200</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>198</v>
-      </c>
-      <c r="E4" t="s" s="0">
+      <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>171</v>
+        <v>165</v>
+      </c>
+      <c r="H4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s" s="0">
-        <v>334</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>337</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>201</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>199</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>171</v>
+        <v>165</v>
+      </c>
+      <c r="H5" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3583,58 +3408,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>326</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>327</v>
-      </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="C3" s="0">
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3">
         <v>14</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>60</v>
+      <c r="D4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3655,31 +3480,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.21875"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>71</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
         <v>68</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3697,9 +3522,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.44140625"/>
-    <col min="2" max="2" customWidth="true" width="16.0"/>
-    <col min="3" max="3" customWidth="true" width="14.21875"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3714,32 +3539,32 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s" s="0">
-        <v>202</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>203</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" t="s" s="0">
-        <v>204</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3759,8 +3584,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
-    <col min="2" max="2" customWidth="true" width="18.77734375"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3775,35 +3600,35 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s" s="0">
-        <v>207</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>205</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>206</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3822,356 +3647,356 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875"/>
-    <col min="4" max="4" customWidth="true" width="19.6640625"/>
-    <col min="7" max="7" customWidth="true" width="10.33203125"/>
-    <col min="8" max="8" customWidth="true" width="16.77734375"/>
-    <col min="9" max="9" customWidth="true" width="16.88671875"/>
-    <col min="11" max="11" customWidth="true" width="13.6640625"/>
-    <col min="12" max="12" customWidth="true" width="15.21875"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>996713</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s" s="0">
-        <v>208</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="L2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
         <v>108</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E2" s="0">
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G3">
         <v>996713</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I3" t="s">
         <v>96</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
         <v>108</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>996713</v>
+      </c>
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" t="s">
         <v>106</v>
       </c>
-      <c r="L2" t="s" s="0">
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s" s="0">
-        <v>209</v>
-      </c>
-      <c r="B3" t="s" s="0">
+      <c r="C5" t="s">
         <v>108</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E3" s="0">
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G5">
         <v>996713</v>
       </c>
-      <c r="H3" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="J3" t="s" s="0">
+      <c r="H5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K5" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
         <v>108</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>996713</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" t="s">
         <v>106</v>
       </c>
-      <c r="L3" t="s" s="0">
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s" s="0">
-        <v>210</v>
-      </c>
-      <c r="B4" t="s" s="0">
+      <c r="C7" t="s">
         <v>108</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E4" s="0">
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G7">
         <v>996713</v>
       </c>
-      <c r="H4" t="s" s="0">
-        <v>90</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>98</v>
-      </c>
-      <c r="J4" t="s" s="0">
+      <c r="H7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
         <v>108</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>996713</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" t="s">
         <v>106</v>
       </c>
-      <c r="L4" t="s" s="0">
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s" s="0">
-        <v>211</v>
-      </c>
-      <c r="B5" t="s" s="0">
+      <c r="C9" t="s">
         <v>108</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E5" s="0">
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G9">
         <v>996713</v>
       </c>
-      <c r="H5" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="K5" t="s" s="0">
+      <c r="H9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" t="s">
         <v>106</v>
-      </c>
-      <c r="L5" t="s" s="0">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s" s="0">
-        <v>212</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E6" s="0">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="K6" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s" s="0">
-        <v>213</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E7" s="0">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="K7" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s" s="0">
-        <v>214</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E8" s="0">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>102</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="K8" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L8" t="s" s="0">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s" s="0">
-        <v>215</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="E9" s="0">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>103</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="K9" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="L9" t="s" s="0">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made in ba page and issues in PO based invoice submission fixed
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\eclipse-workspace\BillHubTest\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291A58F8-8CCF-4B08-88AD-D46717BE3F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D426E1-5B51-43EF-BE06-2C2849D51FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -731,7 +731,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="236">
   <si>
     <t>Medium</t>
   </si>
@@ -1321,30 +1321,6 @@
     <t>testcode_xmwt</t>
   </si>
   <si>
-    <t>TESTINV54120</t>
-  </si>
-  <si>
-    <t>TESTINV57571</t>
-  </si>
-  <si>
-    <t>TESTINV22002</t>
-  </si>
-  <si>
-    <t>TESTINV74948</t>
-  </si>
-  <si>
-    <t>TESTINV16183</t>
-  </si>
-  <si>
-    <t>TESTINV98059</t>
-  </si>
-  <si>
-    <t>TESTINV96987</t>
-  </si>
-  <si>
-    <t>TESTINV73350</t>
-  </si>
-  <si>
     <t>Commercial Name</t>
   </si>
   <si>
@@ -1403,12 +1379,73 @@
   </si>
   <si>
     <t>Anusha Palle</t>
+  </si>
+  <si>
+    <t>TESTINV55027</t>
+  </si>
+  <si>
+    <t>TESTINV16534</t>
+  </si>
+  <si>
+    <t>TESTINV13188</t>
+  </si>
+  <si>
+    <t>TESTINV06960</t>
+  </si>
+  <si>
+    <t>TESTINV34889</t>
+  </si>
+  <si>
+    <t>TESTINV71718</t>
+  </si>
+  <si>
+    <t>TESTINV17878</t>
+  </si>
+  <si>
+    <t>TESTINV53883</t>
+  </si>
+  <si>
+    <t>test_tpmodm</t>
+  </si>
+  <si>
+    <t>test_rnaqbg</t>
+  </si>
+  <si>
+    <t>30003009</t>
+  </si>
+  <si>
+    <t>30004024</t>
+  </si>
+  <si>
+    <t>10006194</t>
+  </si>
+  <si>
+    <t>10001921</t>
+  </si>
+  <si>
+    <t>TESTINV74561</t>
+  </si>
+  <si>
+    <t>TESTINV66739</t>
+  </si>
+  <si>
+    <t>TESTINV06363</t>
+  </si>
+  <si>
+    <t>TESTINV01231</t>
+  </si>
+  <si>
+    <t>TESTINV39084</t>
+  </si>
+  <si>
+    <t>TESTINV47378</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1880,10 +1917,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375"/>
+    <col min="2" max="2" customWidth="true" width="15.21875"/>
+    <col min="3" max="3" customWidth="true" width="15.109375"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1902,12 +1939,12 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C2">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="C2" s="0">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1918,27 +1955,27 @@
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>216</v>
-      </c>
-      <c r="B4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C4">
+      <c r="A4" t="s" s="0">
+        <v>208</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="C4" s="0">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>53</v>
       </c>
     </row>
@@ -1960,9 +1997,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0"/>
+    <col min="2" max="2" customWidth="true" width="18.0"/>
+    <col min="3" max="3" customWidth="true" width="23.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1970,26 +2007,26 @@
         <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>105</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C2" t="s">
-        <v>206</v>
+      <c r="C2" t="s" s="0">
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>207</v>
+      <c r="A3" t="s" s="0">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2008,9 +2045,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" customWidth="true" width="16.44140625"/>
+    <col min="3" max="3" customWidth="true" width="23.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2018,26 +2055,26 @@
         <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>105</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" t="s">
-        <v>206</v>
+        <v>215</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>207</v>
+      <c r="A3" t="s" s="0">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2050,15 +2087,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8206F6E4-0F0D-4202-8599-954FFEEC985A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.44140625"/>
+    <col min="2" max="2" customWidth="true" width="16.5546875"/>
+    <col min="3" max="3" customWidth="true" width="22.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2066,26 +2103,26 @@
         <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>105</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" t="s">
-        <v>206</v>
+        <v>215</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>207</v>
+      <c r="A3" t="s" s="0">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2133,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -2104,15 +2141,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="29.21875"/>
+    <col min="2" max="2" customWidth="true" width="14.6640625"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875"/>
+    <col min="4" max="4" customWidth="true" width="14.44140625"/>
+    <col min="5" max="5" customWidth="true" width="16.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="9" max="9" customWidth="true" width="16.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2145,88 +2182,88 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1022</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>129</v>
       </c>
     </row>
@@ -2246,43 +2283,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.88671875"/>
+    <col min="3" max="3" customWidth="true" width="11.88671875"/>
+    <col min="4" max="4" customWidth="true" width="17.44140625"/>
+    <col min="5" max="5" customWidth="true" width="21.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1022</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>105</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>128</v>
       </c>
     </row>
@@ -2302,10 +2339,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" customWidth="1"/>
-    <col min="14" max="14" width="22.21875" customWidth="1"/>
+    <col min="11" max="11" customWidth="true" width="17.44140625"/>
+    <col min="12" max="12" customWidth="true" width="16.44140625"/>
+    <col min="13" max="13" customWidth="true" width="15.44140625"/>
+    <col min="14" max="14" customWidth="true" width="22.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2353,354 +2390,354 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>996713</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>996713</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>996713</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>996713</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>996713</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>996713</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>996713</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>996713</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" t="s" s="0">
         <v>133</v>
       </c>
     </row>
@@ -2719,16 +2756,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2773,217 +2810,217 @@
       <c r="C2" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="F2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="F2" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J2" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="H3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="H3" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J3" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="B4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" t="s">
-        <v>165</v>
-      </c>
-      <c r="G4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H4" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" t="s">
-        <v>165</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J4" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="B5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="F5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G5" t="s">
-        <v>165</v>
-      </c>
-      <c r="H5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I5" t="s">
-        <v>165</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="F5" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J5" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="C6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H6" t="s">
-        <v>165</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="C6" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="I6" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="A7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="I7" t="s">
-        <v>165</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J7" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="A8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H8" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="I8" t="s">
-        <v>165</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J8" t="s" s="0">
         <v>165</v>
       </c>
     </row>
@@ -2991,63 +3028,63 @@
       <c r="A9" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>165</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="D9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" t="s">
-        <v>165</v>
-      </c>
-      <c r="F9" t="s">
-        <v>165</v>
-      </c>
-      <c r="G9" t="s">
-        <v>165</v>
-      </c>
-      <c r="H9" t="s">
-        <v>165</v>
-      </c>
-      <c r="I9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="D9" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J9" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>165</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C10" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" t="s">
-        <v>165</v>
-      </c>
-      <c r="G10" t="s">
-        <v>165</v>
-      </c>
-      <c r="H10" t="s">
-        <v>165</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="C10" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="I10" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>165</v>
       </c>
     </row>
@@ -3059,23 +3096,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="13.44140625"/>
+    <col min="4" max="4" customWidth="true" width="13.88671875"/>
+    <col min="5" max="5" customWidth="true" width="13.21875"/>
+    <col min="6" max="6" customWidth="true" width="17.77734375"/>
+    <col min="7" max="7" customWidth="true" width="13.88671875"/>
+    <col min="8" max="8" customWidth="true" width="12.0"/>
+    <col min="9" max="9" customWidth="true" width="23.5546875"/>
+    <col min="10" max="10" customWidth="true" width="20.44140625"/>
+    <col min="11" max="11" customWidth="true" width="26.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3115,12 +3152,12 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
       <c r="D2" s="3">
@@ -3132,16 +3169,16 @@
       <c r="F2" s="3">
         <v>5</v>
       </c>
-      <c r="G2" s="3">
-        <v>420</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>3</v>
       </c>
       <c r="K2" s="3">
@@ -3152,10 +3189,10 @@
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>5</v>
       </c>
       <c r="D3" s="3">
@@ -3170,13 +3207,13 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>3</v>
       </c>
       <c r="K3" s="3">
@@ -3185,12 +3222,12 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D4" s="3">
@@ -3202,16 +3239,16 @@
       <c r="F4" s="3">
         <v>5</v>
       </c>
-      <c r="G4" s="3">
-        <v>420</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K4" s="3">
@@ -3235,7 +3272,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
@@ -3243,13 +3280,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="7" width="22.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.109375"/>
+    <col min="2" max="2" customWidth="true" width="12.33203125"/>
+    <col min="3" max="3" customWidth="true" width="16.0"/>
+    <col min="4" max="4" customWidth="true" width="16.5546875"/>
+    <col min="5" max="5" customWidth="true" width="10.77734375"/>
+    <col min="6" max="7" customWidth="true" width="22.109375"/>
+    <col min="8" max="8" customWidth="true" width="12.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3279,19 +3316,19 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>183</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -3300,24 +3337,24 @@
       <c r="G2" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>185</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>180</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -3326,24 +3363,24 @@
       <c r="G3" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>188</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -3352,24 +3389,24 @@
       <c r="G4" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" t="s" s="0">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>189</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>187</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -3378,7 +3415,7 @@
       <c r="G5" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>165</v>
       </c>
     </row>
@@ -3424,27 +3461,27 @@
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" t="s">
-        <v>212</v>
+      <c r="B2" t="s" s="0">
+        <v>203</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>204</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>48</v>
       </c>
     </row>
@@ -3452,13 +3489,13 @@
       <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>59</v>
       </c>
     </row>
@@ -3480,7 +3517,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3492,18 +3529,18 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -3522,9 +3559,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.44140625"/>
+    <col min="2" max="2" customWidth="true" width="16.0"/>
+    <col min="3" max="3" customWidth="true" width="14.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3539,32 +3576,32 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>190</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>39</v>
       </c>
     </row>
@@ -3584,8 +3621,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
+    <col min="2" max="2" customWidth="true" width="18.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3600,35 +3637,35 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>195</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>48</v>
       </c>
     </row>
@@ -3647,14 +3684,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875"/>
+    <col min="4" max="4" customWidth="true" width="19.6640625"/>
+    <col min="7" max="7" customWidth="true" width="10.33203125"/>
+    <col min="8" max="8" customWidth="true" width="16.77734375"/>
+    <col min="9" max="9" customWidth="true" width="16.88671875"/>
+    <col min="11" max="11" customWidth="true" width="13.6640625"/>
+    <col min="12" max="12" customWidth="true" width="15.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3696,306 +3733,306 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>996713</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="J2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K2" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="A3" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>996713</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="J3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="A4" t="s" s="0">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>996713</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="J4" t="s">
-        <v>107</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="J4" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K4" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="A5" t="s" s="0">
+        <v>216</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>996713</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="J5" t="s">
-        <v>107</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="J5" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K5" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="A6" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>996713</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="J6" t="s">
-        <v>107</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="J6" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K6" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="A7" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>996713</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="J7" t="s">
-        <v>107</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="J7" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K7" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>202</v>
-      </c>
-      <c r="B8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="A8" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>996713</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="J8" t="s">
-        <v>107</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="J8" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K8" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="A9" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>996713</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="J9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="J9" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="K9" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes made in config.properties and testng.xml
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\Desktop\billhub new\BillHubTestAutomation\src\main\java\com\billhub\qa\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4890C67E-41A5-49EB-ABB2-3DA4A26EB5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="18" activeTab="20"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreatePaymentRequestForNonPo" sheetId="18" r:id="rId1"/>
@@ -31,7 +37,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,12 +45,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -121,12 +127,12 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="L2" authorId="0">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -155,13 +161,13 @@
 </file>
 
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
     <author>SURAJ PATEL</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -186,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -211,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -236,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -261,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="1">
+    <comment ref="K5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-1200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -311,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -341,12 +347,12 @@
 </file>
 
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -376,12 +382,12 @@
 </file>
 
 <file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -406,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -431,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -461,12 +467,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -490,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -515,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -545,12 +551,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -575,7 +581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -599,7 +605,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -624,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -649,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -674,7 +680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -699,7 +705,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -723,7 +729,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -748,7 +754,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -773,7 +779,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -798,7 +804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -823,7 +829,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -848,7 +854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -873,7 +879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -903,12 +909,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="M2" authorId="0">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -933,7 +939,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -958,7 +964,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -988,12 +994,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="I2" authorId="0">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1018,7 +1024,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1043,7 +1049,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1068,7 +1074,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1098,12 +1104,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1127,7 +1133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1151,7 +1157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1180,12 +1186,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1210,7 +1216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1240,12 +1246,12 @@
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1275,12 +1281,12 @@
 </file>
 
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nishant Gore</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1310,7 +1316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="266">
   <si>
     <t>Medium</t>
   </si>
@@ -1930,42 +1936,12 @@
     <t>/07730/Mar/2023-24</t>
   </si>
   <si>
-    <t>338344</t>
-  </si>
-  <si>
-    <t>980207</t>
-  </si>
-  <si>
-    <t>test_gmpouu</t>
-  </si>
-  <si>
-    <t>test_evuiho</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
     <t>92</t>
   </si>
   <si>
-    <t>test_woyfwr</t>
-  </si>
-  <si>
-    <t>test_vwitul</t>
-  </si>
-  <si>
-    <t>30001804</t>
-  </si>
-  <si>
-    <t>30002638</t>
-  </si>
-  <si>
-    <t>10001674</t>
-  </si>
-  <si>
-    <t>10001229</t>
-  </si>
-  <si>
     <t>test_czsyog</t>
   </si>
   <si>
@@ -2005,36 +1981,6 @@
     <t>854518</t>
   </si>
   <si>
-    <t>TESTINV87077</t>
-  </si>
-  <si>
-    <t>TESTINV55825</t>
-  </si>
-  <si>
-    <t>TESTINV82626</t>
-  </si>
-  <si>
-    <t>TESTINV92622</t>
-  </si>
-  <si>
-    <t>TESTINV94764</t>
-  </si>
-  <si>
-    <t>TESTINV92410</t>
-  </si>
-  <si>
-    <t>TESTINV50017</t>
-  </si>
-  <si>
-    <t>TESTINV16807</t>
-  </si>
-  <si>
-    <t>5100000178</t>
-  </si>
-  <si>
-    <t>MSAEN04/07732/Mar/2023-24</t>
-  </si>
-  <si>
     <t>Memo_number</t>
   </si>
   <si>
@@ -2065,17 +2011,117 @@
     <t>30005631-2023-24-00072</t>
   </si>
   <si>
-    <t xml:space="preserve">	TESTINV97479</t>
-  </si>
-  <si>
     <t>TESTINV7779</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TESTINV58442</t>
+  </si>
+  <si>
+    <t>TESTINV62611</t>
+  </si>
+  <si>
+    <t>TESTINV84676</t>
+  </si>
+  <si>
+    <t>TESTINV91034</t>
+  </si>
+  <si>
+    <t>TESTINV74054</t>
+  </si>
+  <si>
+    <t>TESTINV29084</t>
+  </si>
+  <si>
+    <t>TESTINV74070</t>
+  </si>
+  <si>
+    <t>TESTINV30812</t>
+  </si>
+  <si>
+    <t>5100000179</t>
+  </si>
+  <si>
+    <t>MSAEN04/07734/Mar/2023-24</t>
+  </si>
+  <si>
+    <t>500614</t>
+  </si>
+  <si>
+    <t>440929</t>
+  </si>
+  <si>
+    <t>test_ojxfvp</t>
+  </si>
+  <si>
+    <t>test_tyebhy</t>
+  </si>
+  <si>
+    <t>test_hhfvzo</t>
+  </si>
+  <si>
+    <t>test_oywbwa</t>
+  </si>
+  <si>
+    <t>30007652</t>
+  </si>
+  <si>
+    <t>30006607</t>
+  </si>
+  <si>
+    <t>10004310</t>
+  </si>
+  <si>
+    <t>10002736</t>
+  </si>
+  <si>
+    <t>TESTINV97479</t>
+  </si>
+  <si>
+    <t>test_hsarfh</t>
+  </si>
+  <si>
+    <t>test_nuqqme</t>
+  </si>
+  <si>
+    <t>30009668</t>
+  </si>
+  <si>
+    <t>30001227</t>
+  </si>
+  <si>
+    <t>10006025</t>
+  </si>
+  <si>
+    <t>10001602</t>
+  </si>
+  <si>
+    <t>test_zckoiq</t>
+  </si>
+  <si>
+    <t>test_gdgooc</t>
+  </si>
+  <si>
+    <t>test_mcfjih</t>
+  </si>
+  <si>
+    <t>299216</t>
+  </si>
+  <si>
+    <t>908596</t>
+  </si>
+  <si>
+    <t>550484</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2531,30 +2577,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="27.36328125" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.21875"/>
+    <col min="2" max="2" customWidth="true" width="18.109375"/>
+    <col min="3" max="3" customWidth="true" width="15.0"/>
+    <col min="4" max="4" customWidth="true" width="27.33203125"/>
+    <col min="5" max="5" customWidth="true" width="18.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2571,54 +2617,54 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="E2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>142</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E3" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>142</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>190</v>
       </c>
     </row>
@@ -2630,20 +2676,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
+    <col min="2" max="2" customWidth="true" width="18.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -2654,36 +2700,36 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>48</v>
       </c>
     </row>
@@ -2693,26 +2739,26 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" customWidth="1"/>
-    <col min="7" max="7" width="10.36328125" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" customWidth="1"/>
-    <col min="9" max="9" width="16.90625" customWidth="1"/>
-    <col min="11" max="11" width="13.6328125" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875"/>
+    <col min="4" max="4" customWidth="true" width="19.6640625"/>
+    <col min="7" max="7" customWidth="true" width="10.33203125"/>
+    <col min="8" max="8" customWidth="true" width="16.77734375"/>
+    <col min="9" max="9" customWidth="true" width="16.88671875"/>
+    <col min="11" max="11" customWidth="true" width="13.6640625"/>
+    <col min="12" max="12" customWidth="true" width="15.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2750,307 +2796,307 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>996713</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="J2" t="s">
-        <v>194</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="K2" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0">
+        <v>996713</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s" s="0">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0">
+        <v>996713</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0">
+        <v>996713</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s" s="0">
+        <v>237</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D6" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E3">
+      <c r="E6" s="0">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F6" s="0">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G6" s="0">
         <v>996713</v>
       </c>
-      <c r="H3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="H6" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="J6" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K6" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L6" t="s" s="0">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:12">
+      <c r="A7" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D7" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E4">
+      <c r="E7" s="0">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F7" s="0">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G7" s="0">
         <v>996713</v>
       </c>
-      <c r="H4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="H7" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="J7" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K7" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L7" t="s" s="0">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" t="s" s="0">
+        <v>239</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E5">
+      <c r="E8" s="0">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F8" s="0">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G8" s="0">
         <v>996713</v>
       </c>
-      <c r="H5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" t="s">
-        <v>193</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="H8" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="K8" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L8" t="s" s="0">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>235</v>
-      </c>
-      <c r="B6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="9" spans="1:12">
+      <c r="A9" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D9" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E6">
+      <c r="E9" s="0">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G9" s="0">
         <v>996713</v>
       </c>
-      <c r="H6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" t="s">
-        <v>193</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="H9" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="K9" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>996713</v>
-      </c>
-      <c r="H7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" t="s">
-        <v>193</v>
-      </c>
-      <c r="K7" t="s">
-        <v>104</v>
-      </c>
-      <c r="L7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>237</v>
-      </c>
-      <c r="B8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>996713</v>
-      </c>
-      <c r="H8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J8" t="s">
-        <v>193</v>
-      </c>
-      <c r="K8" t="s">
-        <v>104</v>
-      </c>
-      <c r="L8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>238</v>
-      </c>
-      <c r="B9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>996713</v>
-      </c>
-      <c r="H9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J9" t="s">
-        <v>194</v>
-      </c>
-      <c r="K9" t="s">
-        <v>104</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>105</v>
       </c>
     </row>
@@ -3062,23 +3108,23 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="27.36328125" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.6640625"/>
+    <col min="2" max="2" customWidth="true" width="18.109375"/>
+    <col min="3" max="3" customWidth="true" width="15.0"/>
+    <col min="4" max="4" customWidth="true" width="27.33203125"/>
+    <col min="5" max="5" customWidth="true" width="18.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3095,54 +3141,54 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="B2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B2" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>142</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E3" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>142</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>190</v>
       </c>
     </row>
@@ -3154,22 +3200,22 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0"/>
+    <col min="2" max="2" customWidth="true" width="18.0"/>
+    <col min="3" max="3" customWidth="true" width="23.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
@@ -3183,22 +3229,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s" s="0">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="D2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="D2" t="s" s="0">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s" s="0">
         <v>170</v>
       </c>
     </row>
@@ -3209,22 +3255,22 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" customWidth="true" width="16.44140625"/>
+    <col min="3" max="3" customWidth="true" width="23.77734375"/>
+    <col min="4" max="4" customWidth="true" width="22.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
@@ -3238,22 +3284,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s" s="0">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s" s="0">
         <v>170</v>
       </c>
     </row>
@@ -3264,22 +3310,22 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.44140625"/>
+    <col min="2" max="2" customWidth="true" width="16.5546875"/>
+    <col min="3" max="3" customWidth="true" width="22.77734375"/>
+    <col min="4" max="4" customWidth="true" width="22.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
@@ -3293,22 +3339,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s" s="0">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>1900000038</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s" s="0">
         <v>170</v>
       </c>
     </row>
@@ -3320,27 +3366,27 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="29.21875"/>
+    <col min="2" max="2" customWidth="true" width="14.6640625"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875"/>
+    <col min="4" max="4" customWidth="true" width="14.44140625"/>
+    <col min="5" max="5" customWidth="true" width="16.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="9" max="9" customWidth="true" width="16.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -3369,89 +3415,89 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1022</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>122</v>
       </c>
     </row>
@@ -3462,52 +3508,52 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="14.90625" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.88671875"/>
+    <col min="3" max="3" customWidth="true" width="11.88671875"/>
+    <col min="4" max="4" customWidth="true" width="17.44140625"/>
+    <col min="5" max="5" customWidth="true" width="21.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" s="0">
         <v>1022</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>104</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>121</v>
       </c>
     </row>
@@ -3518,22 +3564,22 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" width="17.453125" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" customWidth="1"/>
-    <col min="13" max="13" width="15.453125" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" customWidth="1"/>
+    <col min="11" max="11" customWidth="true" width="17.44140625"/>
+    <col min="12" max="12" customWidth="true" width="16.44140625"/>
+    <col min="13" max="13" customWidth="true" width="15.44140625"/>
+    <col min="14" max="14" customWidth="true" width="22.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -3577,355 +3623,355 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>996713</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>996713</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>996713</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14">
+      <c r="A5" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>996713</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>996713</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:14">
+      <c r="A7" t="s" s="0">
         <v>201</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>996713</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:14">
+      <c r="A8" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>996713</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" t="s" s="0">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>996713</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" t="s" s="0">
         <v>126</v>
       </c>
     </row>
@@ -3936,441 +3982,441 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.21875"/>
+    <col min="2" max="2" customWidth="true" width="18.21875"/>
+    <col min="3" max="3" customWidth="true" width="15.44140625"/>
+    <col min="4" max="4" customWidth="true" width="16.6640625"/>
+    <col min="5" max="5" customWidth="true" width="12.77734375"/>
+    <col min="6" max="6" customWidth="true" width="15.21875"/>
+    <col min="7" max="7" customWidth="true" width="13.77734375"/>
+    <col min="8" max="8" customWidth="true" width="16.44140625"/>
+    <col min="10" max="10" customWidth="true" width="16.0"/>
+    <col min="12" max="12" customWidth="true" width="18.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>172</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="F2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2">
+      <c r="F2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K2" s="0">
         <v>996713</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="H3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" t="s">
-        <v>142</v>
-      </c>
-      <c r="J3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K3">
+      <c r="H3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K3" s="0">
         <v>996713</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="F4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K4">
+      <c r="F4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K4" s="0">
         <v>996713</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:13">
+      <c r="A5" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="B5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="F5" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K5">
+      <c r="F5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K5" s="0">
         <v>996719</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:13">
+      <c r="A6" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="C6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="C6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I6" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="0">
         <v>996713</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G7" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s" s="0">
         <v>142</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I7" t="s">
-        <v>142</v>
-      </c>
-      <c r="J7" t="s">
-        <v>142</v>
-      </c>
-      <c r="K7">
+      <c r="I7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K7" s="0">
         <v>996713</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" t="s">
-        <v>142</v>
-      </c>
-      <c r="G8" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G8" t="s" s="0">
         <v>142</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="I8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J8" t="s">
-        <v>142</v>
-      </c>
-      <c r="K8">
+      <c r="I8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K8" s="0">
         <v>996713</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:13">
+      <c r="A9" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="D9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" t="s">
-        <v>142</v>
-      </c>
-      <c r="G9" t="s">
-        <v>142</v>
-      </c>
-      <c r="H9" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" t="s">
-        <v>142</v>
-      </c>
-      <c r="J9" t="s">
-        <v>142</v>
-      </c>
-      <c r="K9">
+      <c r="D9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K9" s="0">
         <v>996713</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="C10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" t="s">
-        <v>142</v>
-      </c>
-      <c r="H10" t="s">
-        <v>142</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="C10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I10" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="J10" t="s">
-        <v>142</v>
-      </c>
-      <c r="K10">
+      <c r="J10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="K10" s="0">
         <v>996713</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="0">
         <v>1500000081</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="0">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1"/>
-    <hyperlink ref="H8" r:id="rId2"/>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="H8" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId3"/>
@@ -4378,100 +4424,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.77734375"/>
+    <col min="2" max="2" customWidth="true" width="15.0"/>
+    <col min="3" max="3" customWidth="true" width="14.6640625"/>
+    <col min="4" max="4" customWidth="true" width="14.88671875"/>
+    <col min="5" max="5" customWidth="true" width="16.33203125"/>
+    <col min="6" max="6" customWidth="true" width="16.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="13" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="D2" t="s">
-        <v>248</v>
+        <v>226</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>228</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>142</v>
       </c>
     </row>
@@ -4484,22 +4530,22 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.21875"/>
+    <col min="2" max="2" customWidth="true" width="18.88671875"/>
+    <col min="3" max="3" customWidth="true" width="22.6640625"/>
+    <col min="4" max="4" customWidth="true" width="22.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
@@ -4513,22 +4559,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s" s="0">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s" s="0">
         <v>170</v>
       </c>
     </row>
@@ -4539,100 +4585,100 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.90625" customWidth="1"/>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.88671875"/>
+    <col min="2" max="2" customWidth="true" width="20.33203125"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125"/>
+    <col min="4" max="4" customWidth="true" width="13.21875"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625"/>
+    <col min="6" max="6" customWidth="true" width="20.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="13" t="s">
         <v>177</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="D2" t="s">
-        <v>248</v>
+        <v>226</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>228</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>142</v>
       </c>
     </row>
@@ -4644,22 +4690,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375"/>
+    <col min="2" max="2" customWidth="true" width="15.21875"/>
+    <col min="3" max="3" customWidth="true" width="15.109375"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -4673,79 +4719,79 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>243</v>
+      </c>
+      <c r="C2" s="0">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>209</v>
-      </c>
-      <c r="B4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="C4" s="0">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.77734375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.77734375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.109375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -4777,7 +4823,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="7" t="s">
         <v>138</v>
       </c>
@@ -4787,281 +4833,281 @@
       <c r="C2" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="F2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="F2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="H3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" t="s">
-        <v>142</v>
-      </c>
-      <c r="J3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="H3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="B5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="F5" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="C6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="C6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I6" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G7" t="s">
-        <v>142</v>
-      </c>
-      <c r="H7" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="I7" t="s">
-        <v>142</v>
-      </c>
-      <c r="J7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" t="s">
-        <v>142</v>
-      </c>
-      <c r="G8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I7" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1">
+      <c r="A8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H8" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="I8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I8" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>142</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" t="s">
-        <v>142</v>
-      </c>
-      <c r="G9" t="s">
-        <v>142</v>
-      </c>
-      <c r="H9" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" t="s">
-        <v>142</v>
-      </c>
-      <c r="J9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="D9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s" s="0">
         <v>142</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" t="s">
-        <v>142</v>
-      </c>
-      <c r="H10" t="s">
-        <v>142</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="C10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="I10" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>142</v>
       </c>
     </row>
@@ -5072,27 +5118,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="23.54296875" customWidth="1"/>
-    <col min="10" max="10" width="20.453125" customWidth="1"/>
-    <col min="11" max="11" width="26.36328125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="13.44140625"/>
+    <col min="4" max="4" customWidth="true" width="13.88671875"/>
+    <col min="5" max="5" customWidth="true" width="13.21875"/>
+    <col min="6" max="6" customWidth="true" width="17.77734375"/>
+    <col min="7" max="7" customWidth="true" width="13.88671875"/>
+    <col min="8" max="8" customWidth="true" width="12.0"/>
+    <col min="9" max="9" customWidth="true" width="23.5546875"/>
+    <col min="10" max="10" customWidth="true" width="20.44140625"/>
+    <col min="11" max="11" customWidth="true" width="26.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -5127,14 +5173,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>254</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
       <c r="D2" s="3">
@@ -5147,29 +5193,29 @@
         <v>5</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="H2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>3</v>
       </c>
       <c r="K2" s="3">
         <v>9876543210</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>5</v>
       </c>
       <c r="D3" s="3">
@@ -5184,27 +5230,27 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>3</v>
       </c>
       <c r="K3" s="3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D4" s="3">
@@ -5217,30 +5263,30 @@
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="H4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>8</v>
       </c>
       <c r="K4" s="3">
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13">
       <c r="A5" s="3"/>
       <c r="K5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId4"/>
@@ -5248,25 +5294,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" customWidth="1"/>
-    <col min="6" max="7" width="22.08984375" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.109375"/>
+    <col min="2" max="2" customWidth="true" width="12.33203125"/>
+    <col min="3" max="3" customWidth="true" width="16.0"/>
+    <col min="4" max="4" customWidth="true" width="16.5546875"/>
+    <col min="5" max="5" customWidth="true" width="10.77734375"/>
+    <col min="6" max="7" customWidth="true" width="22.109375"/>
+    <col min="8" max="8" customWidth="true" width="12.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -5292,20 +5338,20 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -5314,24 +5360,24 @@
       <c r="G2" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>161</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>162</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>157</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -5340,24 +5386,24 @@
       <c r="G3" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="H3" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>163</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -5366,24 +5412,24 @@
       <c r="G4" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="H4" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -5392,17 +5438,17 @@
       <c r="G5" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>142</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -5411,16 +5457,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -5434,70 +5480,70 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" t="s">
-        <v>211</v>
+      <c r="B2" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>207</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
@@ -5505,19 +5551,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B2" t="s" s="0">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -5527,21 +5573,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.44140625"/>
+    <col min="2" max="2" customWidth="true" width="16.0"/>
+    <col min="3" max="3" customWidth="true" width="14.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -5552,33 +5598,33 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="4" spans="1:3">
+      <c r="B4" t="s" s="0">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code refactored and finalised
</commit_message>
<xml_diff>
--- a/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
+++ b/src/main/java/com/billhub/qa/testdata/BillHubTestdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha\Desktop\billhub new\BillHubTestAutomation\src\main\java\com\billhub\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4890C67E-41A5-49EB-ABB2-3DA4A26EB5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F04028-1452-4017-90AF-B14B45DB3741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreatePaymentRequestForNonPo" sheetId="18" r:id="rId1"/>
@@ -37,7 +37,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1316,7 +1316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="255">
   <si>
     <t>Medium</t>
   </si>
@@ -1942,24 +1942,6 @@
     <t>92</t>
   </si>
   <si>
-    <t>test_czsyog</t>
-  </si>
-  <si>
-    <t>test_pszgha</t>
-  </si>
-  <si>
-    <t>test_xepklo</t>
-  </si>
-  <si>
-    <t>232862</t>
-  </si>
-  <si>
-    <t>456954</t>
-  </si>
-  <si>
-    <t>934173</t>
-  </si>
-  <si>
     <t>XD</t>
   </si>
   <si>
@@ -2011,9 +1993,6 @@
     <t>30005631-2023-24-00072</t>
   </si>
   <si>
-    <t>TESTINV7779</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -2059,24 +2038,6 @@
     <t>test_tyebhy</t>
   </si>
   <si>
-    <t>test_hhfvzo</t>
-  </si>
-  <si>
-    <t>test_oywbwa</t>
-  </si>
-  <si>
-    <t>30007652</t>
-  </si>
-  <si>
-    <t>30006607</t>
-  </si>
-  <si>
-    <t>10004310</t>
-  </si>
-  <si>
-    <t>10002736</t>
-  </si>
-  <si>
     <t>TESTINV97479</t>
   </si>
   <si>
@@ -2114,13 +2075,18 @@
   </si>
   <si>
     <t>550484</t>
+  </si>
+  <si>
+    <t>30005574-2023-24-00009</t>
+  </si>
+  <si>
+    <t>TESTINV72213</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -2593,11 +2559,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.21875"/>
-    <col min="2" max="2" customWidth="true" width="18.109375"/>
-    <col min="3" max="3" customWidth="true" width="15.0"/>
-    <col min="4" max="4" customWidth="true" width="27.33203125"/>
-    <col min="5" max="5" customWidth="true" width="18.88671875"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2618,53 +2584,53 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>181</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>204</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>196</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>205</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>105</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
         <v>142</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
         <v>142</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2685,8 +2651,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.5546875"/>
-    <col min="2" max="2" customWidth="true" width="18.77734375"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2701,35 +2667,35 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s" s="0">
-        <v>219</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>217</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>218</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2748,14 +2714,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875"/>
-    <col min="4" max="4" customWidth="true" width="19.6640625"/>
-    <col min="7" max="7" customWidth="true" width="10.33203125"/>
-    <col min="8" max="8" customWidth="true" width="16.77734375"/>
-    <col min="9" max="9" customWidth="true" width="16.88671875"/>
-    <col min="11" max="11" customWidth="true" width="13.6640625"/>
-    <col min="12" max="12" customWidth="true" width="15.21875"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2797,306 +2763,306 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>996713</v>
+      </c>
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>996713</v>
+      </c>
+      <c r="H3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s">
+        <v>193</v>
+      </c>
+      <c r="K3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>996713</v>
+      </c>
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" t="s">
+        <v>225</v>
+      </c>
+      <c r="K4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>996713</v>
+      </c>
+      <c r="H5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>996713</v>
+      </c>
+      <c r="H6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" t="s">
+        <v>193</v>
+      </c>
+      <c r="K6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>996713</v>
+      </c>
+      <c r="H7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" t="s">
+        <v>193</v>
+      </c>
+      <c r="K7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>996713</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
         <v>233</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B9" t="s">
         <v>106</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C9" t="s">
         <v>191</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D9" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G9">
         <v>996713</v>
       </c>
-      <c r="H2" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="J2" t="s" s="0">
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" t="s">
         <v>106</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K9" t="s">
         <v>104</v>
       </c>
-      <c r="L2" t="s" s="0">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s" s="0">
-        <v>234</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>193</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>191</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E3" s="0">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>87</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>193</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="L3" t="s" s="0">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s" s="0">
-        <v>235</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>232</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>191</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E4" s="0">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>232</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="L4" t="s" s="0">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s" s="0">
-        <v>236</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>191</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E5" s="0">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="K5" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="L5" t="s" s="0">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s" s="0">
-        <v>237</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>193</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>191</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E6" s="0">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>90</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>98</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>193</v>
-      </c>
-      <c r="K6" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s" s="0">
-        <v>238</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>193</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>191</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E7" s="0">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>193</v>
-      </c>
-      <c r="K7" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s" s="0">
-        <v>239</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>191</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E8" s="0">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="K8" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="L8" t="s" s="0">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s" s="0">
-        <v>240</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>191</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="E9" s="0">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0">
-        <v>996713</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="K9" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="L9" t="s" s="0">
+      <c r="L9" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3117,11 +3083,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.6640625"/>
-    <col min="2" max="2" customWidth="true" width="18.109375"/>
-    <col min="3" max="3" customWidth="true" width="15.0"/>
-    <col min="4" max="4" customWidth="true" width="27.33203125"/>
-    <col min="5" max="5" customWidth="true" width="18.88671875"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3142,53 +3108,53 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>146</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>241</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>233</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>242</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>105</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
         <v>142</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
         <v>142</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3209,10 +3175,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.0"/>
-    <col min="2" max="2" customWidth="true" width="18.0"/>
-    <col min="3" max="3" customWidth="true" width="23.77734375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3230,21 +3196,21 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>169</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>241</v>
+      <c r="D2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3264,10 +3230,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="2" max="2" customWidth="true" width="16.44140625"/>
-    <col min="3" max="3" customWidth="true" width="23.77734375"/>
-    <col min="4" max="4" customWidth="true" width="22.44140625"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3285,21 +3251,21 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>169</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3319,10 +3285,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.44140625"/>
-    <col min="2" max="2" customWidth="true" width="16.5546875"/>
-    <col min="3" max="3" customWidth="true" width="22.77734375"/>
-    <col min="4" max="4" customWidth="true" width="22.6640625"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3340,21 +3306,21 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>1900000038</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3367,7 +3333,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -3375,15 +3341,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.21875"/>
-    <col min="2" max="2" customWidth="true" width="14.6640625"/>
-    <col min="3" max="3" customWidth="true" width="15.5546875"/>
-    <col min="4" max="4" customWidth="true" width="14.44140625"/>
-    <col min="5" max="5" customWidth="true" width="16.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="9" max="9" customWidth="true" width="16.33203125"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3416,88 +3382,88 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>107</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>104</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>1022</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>82</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>114</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>111</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>129</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>129</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>129</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>129</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>130</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>130</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>130</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>130</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>131</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>192</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>104</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>131</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>192</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>104</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3517,43 +3483,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.88671875"/>
-    <col min="3" max="3" customWidth="true" width="11.88671875"/>
-    <col min="4" max="4" customWidth="true" width="17.44140625"/>
-    <col min="5" max="5" customWidth="true" width="21.77734375"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>116</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>117</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>118</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1022</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>120</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>104</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3573,10 +3539,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" customWidth="true" width="17.44140625"/>
-    <col min="12" max="12" customWidth="true" width="16.44140625"/>
-    <col min="13" max="13" customWidth="true" width="15.44140625"/>
-    <col min="14" max="14" customWidth="true" width="22.21875"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
+    <col min="14" max="14" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3624,354 +3590,354 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>196</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>193</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>191</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>996713</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>86</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>94</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>193</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>104</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>122</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>125</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>197</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>193</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>191</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>996713</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>87</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>95</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>193</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>104</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>122</v>
       </c>
-      <c r="M3" t="s" s="0">
+      <c r="M3" t="s">
         <v>127</v>
       </c>
-      <c r="N3" t="s" s="0">
+      <c r="N3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>198</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>194</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>191</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>996713</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>88</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="I4" t="s">
         <v>96</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>194</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K4" t="s">
         <v>104</v>
       </c>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>122</v>
       </c>
-      <c r="M4" t="s" s="0">
+      <c r="M4" t="s">
         <v>127</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>199</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>193</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>191</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>996713</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>89</v>
       </c>
-      <c r="I5" t="s" s="0">
+      <c r="I5" t="s">
         <v>97</v>
       </c>
-      <c r="J5" t="s" s="0">
+      <c r="J5" t="s">
         <v>193</v>
       </c>
-      <c r="K5" t="s" s="0">
+      <c r="K5" t="s">
         <v>104</v>
       </c>
-      <c r="L5" t="s" s="0">
+      <c r="L5" t="s">
         <v>122</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>128</v>
       </c>
-      <c r="N5" t="s" s="0">
+      <c r="N5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>200</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>106</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>191</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>996713</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>90</v>
       </c>
-      <c r="I6" t="s" s="0">
+      <c r="I6" t="s">
         <v>98</v>
       </c>
-      <c r="J6" t="s" s="0">
+      <c r="J6" t="s">
         <v>106</v>
       </c>
-      <c r="K6" t="s" s="0">
+      <c r="K6" t="s">
         <v>104</v>
       </c>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>122</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>128</v>
       </c>
-      <c r="N6" t="s" s="0">
+      <c r="N6" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>201</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>106</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>191</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>996713</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="H7" t="s">
         <v>91</v>
       </c>
-      <c r="I7" t="s" s="0">
+      <c r="I7" t="s">
         <v>99</v>
       </c>
-      <c r="J7" t="s" s="0">
+      <c r="J7" t="s">
         <v>106</v>
       </c>
-      <c r="K7" t="s" s="0">
+      <c r="K7" t="s">
         <v>104</v>
       </c>
-      <c r="L7" t="s" s="0">
+      <c r="L7" t="s">
         <v>122</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>128</v>
       </c>
-      <c r="N7" t="s" s="0">
+      <c r="N7" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>202</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>106</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>191</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>996713</v>
       </c>
-      <c r="H8" t="s" s="0">
+      <c r="H8" t="s">
         <v>92</v>
       </c>
-      <c r="I8" t="s" s="0">
+      <c r="I8" t="s">
         <v>100</v>
       </c>
-      <c r="J8" t="s" s="0">
+      <c r="J8" t="s">
         <v>106</v>
       </c>
-      <c r="K8" t="s" s="0">
+      <c r="K8" t="s">
         <v>104</v>
       </c>
-      <c r="L8" t="s" s="0">
+      <c r="L8" t="s">
         <v>122</v>
       </c>
-      <c r="M8" t="s" s="0">
+      <c r="M8" t="s">
         <v>125</v>
       </c>
-      <c r="N8" t="s" s="0">
+      <c r="N8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>203</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>106</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>191</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>996713</v>
       </c>
-      <c r="H9" t="s" s="0">
+      <c r="H9" t="s">
         <v>93</v>
       </c>
-      <c r="I9" t="s" s="0">
+      <c r="I9" t="s">
         <v>101</v>
       </c>
-      <c r="J9" t="s" s="0">
+      <c r="J9" t="s">
         <v>106</v>
       </c>
-      <c r="K9" t="s" s="0">
+      <c r="K9" t="s">
         <v>104</v>
       </c>
-      <c r="L9" t="s" s="0">
+      <c r="L9" t="s">
         <v>122</v>
       </c>
-      <c r="M9" t="s" s="0">
+      <c r="M9" t="s">
         <v>125</v>
       </c>
-      <c r="N9" t="s" s="0">
+      <c r="N9" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3991,56 +3957,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.21875"/>
-    <col min="2" max="2" customWidth="true" width="18.21875"/>
-    <col min="3" max="3" customWidth="true" width="15.44140625"/>
-    <col min="4" max="4" customWidth="true" width="16.6640625"/>
-    <col min="5" max="5" customWidth="true" width="12.77734375"/>
-    <col min="6" max="6" customWidth="true" width="15.21875"/>
-    <col min="7" max="7" customWidth="true" width="13.77734375"/>
-    <col min="8" max="8" customWidth="true" width="16.44140625"/>
-    <col min="10" max="10" customWidth="true" width="16.0"/>
-    <col min="12" max="12" customWidth="true" width="18.77734375"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>132</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>133</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>134</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>135</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>137</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="K1" t="s">
         <v>171</v>
       </c>
-      <c r="L1" t="s" s="0">
+      <c r="L1" t="s">
         <v>172</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4048,40 +4014,40 @@
       <c r="A2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>175</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>141</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>141</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K2" s="0">
+      <c r="F2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2">
         <v>996713</v>
       </c>
-      <c r="L2" s="0">
+      <c r="L2">
         <v>1500000081</v>
       </c>
-      <c r="M2" s="0">
+      <c r="M2">
         <v>2</v>
       </c>
     </row>
@@ -4089,327 +4055,327 @@
       <c r="A3" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
         <v>104</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>105</v>
       </c>
-      <c r="H3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K3" s="0">
+      <c r="H3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3">
         <v>996713</v>
       </c>
-      <c r="L3" s="0">
+      <c r="L3">
         <v>1500000081</v>
       </c>
-      <c r="M3" s="0">
+      <c r="M3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>177</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
         <v>141</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>141</v>
       </c>
-      <c r="F4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K4" s="0">
+      <c r="F4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4">
         <v>996713</v>
       </c>
-      <c r="L4" s="0">
+      <c r="L4">
         <v>1500000081</v>
       </c>
-      <c r="M4" s="0">
+      <c r="M4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" t="s">
         <v>141</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>141</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K5" s="0">
+      <c r="F5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" t="s">
+        <v>142</v>
+      </c>
+      <c r="J5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5">
         <v>996719</v>
       </c>
-      <c r="L5" s="0">
+      <c r="L5">
         <v>1500000081</v>
       </c>
-      <c r="M5" s="0">
+      <c r="M5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>179</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>180</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I6" t="s" s="0">
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" t="s">
         <v>181</v>
       </c>
-      <c r="J6" t="s" s="0">
+      <c r="J6" t="s">
         <v>122</v>
       </c>
-      <c r="K6" s="0">
+      <c r="K6">
         <v>996713</v>
       </c>
-      <c r="L6" s="0">
+      <c r="L6">
         <v>1500000081</v>
       </c>
-      <c r="M6" s="0">
+      <c r="M6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G7" t="s" s="0">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s">
         <v>142</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K7" s="0">
+      <c r="I7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7">
         <v>996713</v>
       </c>
-      <c r="L7" s="0">
+      <c r="L7">
         <v>1500000081</v>
       </c>
-      <c r="M7" s="0">
+      <c r="M7">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G8" t="s" s="0">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" t="s">
         <v>142</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="I8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K8" s="0">
+      <c r="I8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8">
         <v>996713</v>
       </c>
-      <c r="L8" s="0">
+      <c r="L8">
         <v>1500000081</v>
       </c>
-      <c r="M8" s="0">
+      <c r="M8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>184</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s">
         <v>150</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K9" s="0">
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9">
         <v>996713</v>
       </c>
-      <c r="L9" s="0">
+      <c r="L9">
         <v>1500000081</v>
       </c>
-      <c r="M9" s="0">
+      <c r="M9">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B10" t="s" s="0">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" t="s">
         <v>151</v>
       </c>
-      <c r="C10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I10" t="s" s="0">
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" t="s">
         <v>152</v>
       </c>
-      <c r="J10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="K10" s="0">
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10">
         <v>996713</v>
       </c>
-      <c r="L10" s="0">
+      <c r="L10">
         <v>1500000081</v>
       </c>
-      <c r="M10" s="0">
+      <c r="M10">
         <v>4</v>
       </c>
     </row>
@@ -4427,35 +4393,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.77734375"/>
-    <col min="2" max="2" customWidth="true" width="15.0"/>
-    <col min="3" max="3" customWidth="true" width="14.6640625"/>
-    <col min="4" max="4" customWidth="true" width="14.88671875"/>
-    <col min="5" max="5" customWidth="true" width="16.33203125"/>
-    <col min="6" max="6" customWidth="true" width="16.44140625"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>133</v>
@@ -4463,61 +4429,61 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="13" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>228</v>
+        <v>220</v>
+      </c>
+      <c r="D2" t="s">
+        <v>222</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F4" t="s" s="0">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4539,10 +4505,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.21875"/>
-    <col min="2" max="2" customWidth="true" width="18.88671875"/>
-    <col min="3" max="3" customWidth="true" width="22.6640625"/>
-    <col min="4" max="4" customWidth="true" width="22.0"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4560,21 +4526,21 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>169</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4588,35 +4554,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.88671875"/>
-    <col min="2" max="2" customWidth="true" width="20.33203125"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125"/>
-    <col min="4" max="4" customWidth="true" width="13.21875"/>
-    <col min="5" max="5" customWidth="true" width="13.44140625"/>
-    <col min="6" max="6" customWidth="true" width="20.21875"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>133</v>
@@ -4624,41 +4590,41 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="13" t="s">
-        <v>177</v>
+        <v>253</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>228</v>
+        <v>220</v>
+      </c>
+      <c r="D2" t="s">
+        <v>222</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4666,19 +4632,19 @@
       <c r="A4" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4699,10 +4665,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375"/>
-    <col min="2" max="2" customWidth="true" width="15.21875"/>
-    <col min="3" max="3" customWidth="true" width="15.109375"/>
-    <col min="4" max="4" customWidth="true" width="16.88671875"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4721,12 +4687,12 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>243</v>
-      </c>
-      <c r="C2" s="0">
+        <v>238</v>
+      </c>
+      <c r="B2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -4737,27 +4703,27 @@
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s" s="0">
-        <v>246</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>244</v>
-      </c>
-      <c r="C4" s="0">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4779,16 +4745,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.77734375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.77734375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.77734375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.109375"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4833,217 +4799,217 @@
       <c r="C2" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>141</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>141</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
         <v>104</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>143</v>
       </c>
-      <c r="H3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J3" t="s" s="0">
+      <c r="H3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>114</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>121</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" t="s">
         <v>141</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>141</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J5" t="s" s="0">
+      <c r="F5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" t="s">
+        <v>142</v>
+      </c>
+      <c r="J5" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>144</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>145</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I6" t="s" s="0">
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" t="s">
         <v>146</v>
       </c>
-      <c r="J6" t="s" s="0">
+      <c r="J6" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H7" t="s" s="0">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7" t="s">
         <v>147</v>
       </c>
-      <c r="I7" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J7" t="s" s="0">
+      <c r="I7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H8" t="s" s="0">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H8" t="s">
         <v>148</v>
       </c>
-      <c r="I8" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J8" t="s" s="0">
+      <c r="I8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5051,63 +5017,63 @@
       <c r="A9" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>142</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="J9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="I10" t="s" s="0">
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" t="s">
         <v>152</v>
       </c>
-      <c r="J10" t="s" s="0">
+      <c r="J10" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5119,7 +5085,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -5127,15 +5093,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.44140625"/>
-    <col min="4" max="4" customWidth="true" width="13.88671875"/>
-    <col min="5" max="5" customWidth="true" width="13.21875"/>
-    <col min="6" max="6" customWidth="true" width="17.77734375"/>
-    <col min="7" max="7" customWidth="true" width="13.88671875"/>
-    <col min="8" max="8" customWidth="true" width="12.0"/>
-    <col min="9" max="9" customWidth="true" width="23.5546875"/>
-    <col min="10" max="10" customWidth="true" width="20.44140625"/>
-    <col min="11" max="11" customWidth="true" width="26.33203125"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -5175,12 +5141,12 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="C2" t="s" s="0">
+        <v>243</v>
+      </c>
+      <c r="B2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3">
@@ -5193,15 +5159,15 @@
         <v>5</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="H2" t="s" s="0">
+        <v>245</v>
+      </c>
+      <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="3">
@@ -5212,10 +5178,10 @@
       <c r="A3" s="3">
         <v>429</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3">
@@ -5230,13 +5196,13 @@
       <c r="G3" s="3">
         <v>420</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="3">
@@ -5245,12 +5211,12 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>255</v>
-      </c>
-      <c r="C4" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3">
@@ -5263,15 +5229,15 @@
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H4" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="H4" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="3">
@@ -5295,7 +5261,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C5"/>
@@ -5303,13 +5269,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.109375"/>
-    <col min="2" max="2" customWidth="true" width="12.33203125"/>
-    <col min="3" max="3" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" width="16.5546875"/>
-    <col min="5" max="5" customWidth="true" width="10.77734375"/>
-    <col min="6" max="7" customWidth="true" width="22.109375"/>
-    <col min="8" max="8" customWidth="true" width="12.21875"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5339,19 +5305,19 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s" s="0">
-        <v>260</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
         <v>159</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>160</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -5360,24 +5326,24 @@
       <c r="G2" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="s" s="0">
-        <v>261</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>264</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" t="s">
         <v>161</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>162</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>157</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -5386,24 +5352,24 @@
       <c r="G3" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>165</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>163</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -5412,24 +5378,24 @@
       <c r="G4" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s" s="0">
-        <v>262</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>265</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="A5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" t="s">
         <v>166</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>164</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -5438,7 +5404,7 @@
       <c r="G5" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5484,10 +5450,10 @@
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>206</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>207</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -5495,16 +5461,16 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>14</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -5512,13 +5478,13 @@
       <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5540,7 +5506,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.21875"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5552,18 +5518,18 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>220</v>
+      <c r="B2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -5582,9 +5548,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.44140625"/>
-    <col min="2" max="2" customWidth="true" width="16.0"/>
-    <col min="3" max="3" customWidth="true" width="14.21875"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5599,32 +5565,32 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s" s="0">
-        <v>214</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>215</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" t="s" s="0">
-        <v>216</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>